<commit_message>
🚧emparejamiento auto, faltan columnas salida
</commit_message>
<xml_diff>
--- a/recursos/EmparejamientoFINAL.xlsx
+++ b/recursos/EmparejamientoFINAL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\OneDrive\Documents\7 semestre\Sistema-TuGestor\recursos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\Sistema-TuGestor\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB653F65-4D7A-4929-8D6B-AE8151877B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44994990-2746-4FD1-9077-A5F8535FAD76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="670" xr2:uid="{FD9F6918-DD5F-4EFB-A5DA-81B3D2DC95CD}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14640" windowHeight="16305" tabRatio="670" xr2:uid="{FD9F6918-DD5F-4EFB-A5DA-81B3D2DC95CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Emparejamiento" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="169">
   <si>
     <t>1.id</t>
   </si>
@@ -513,15 +513,6 @@
     <t>Colegio San Agustin</t>
   </si>
   <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
     <t>Prueba3@pruebmail.com</t>
   </si>
   <si>
@@ -589,6 +580,18 @@
   </si>
   <si>
     <t>Institucion camilo vargas</t>
+  </si>
+  <si>
+    <t>80 horas - 1 tutorado</t>
+  </si>
+  <si>
+    <t>40 horas - 1 tutorado</t>
+  </si>
+  <si>
+    <t>80 horas - 2 tutorado</t>
+  </si>
+  <si>
+    <t>100 horas - 1 tutorado</t>
   </si>
 </sst>
 </file>
@@ -2395,8 +2398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D120C5C-D1E3-40C4-B4D7-C7D7020D0451}">
   <dimension ref="A1:AZ57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2444,7 +2447,7 @@
         <v>23</v>
       </c>
       <c r="J1" s="31" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="K1" s="11" t="s">
         <v>24</v>
@@ -2501,10 +2504,10 @@
         <v>14</v>
       </c>
       <c r="AC1" s="32" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="AD1" s="33" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="AE1" s="13" t="s">
         <v>45</v>
@@ -2561,10 +2564,10 @@
         <v>43</v>
       </c>
       <c r="AW1" s="32" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="AX1" s="33" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="AY1" s="9" t="s">
         <v>44</v>
@@ -2596,13 +2599,13 @@
         <v>46</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
       <c r="I2" s="16">
         <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K2" s="17" t="s">
         <v>70</v>
@@ -2659,10 +2662,10 @@
         <v>3.1</v>
       </c>
       <c r="AC2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="AD2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AE2" s="17" t="s">
         <v>130</v>
@@ -2683,7 +2686,7 @@
         <v>73</v>
       </c>
       <c r="AK2" s="17" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="AL2" s="29">
         <v>2.2999999999999998</v>
@@ -2719,10 +2722,10 @@
         <v>3.2</v>
       </c>
       <c r="AW2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="AX2" s="29" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AY2" s="21" t="s">
         <v>59</v>
@@ -2751,16 +2754,16 @@
         <v>69</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>143</v>
+        <v>166</v>
       </c>
       <c r="I3" s="19" t="s">
         <v>80</v>
       </c>
       <c r="J3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K3" t="s">
         <v>112</v>
@@ -2781,7 +2784,7 @@
         <v>121</v>
       </c>
       <c r="Q3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R3" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
@@ -2789,31 +2792,31 @@
       </c>
       <c r="S3" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>0.9</v>
+        <v>3</v>
       </c>
       <c r="T3" s="28">
         <f t="shared" ref="T3:AB10" ca="1" si="0">ROUND(RAND()*5,1)</f>
-        <v>0.5</v>
+        <v>2.1</v>
       </c>
       <c r="U3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="V3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8</v>
+        <v>3.7</v>
       </c>
       <c r="W3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4000000000000004</v>
+        <v>1.5</v>
       </c>
       <c r="X3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2</v>
+        <v>2.8</v>
       </c>
       <c r="Y3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2</v>
+        <v>0.7</v>
       </c>
       <c r="Z3" s="28">
         <f t="shared" ca="1" si="0"/>
@@ -2821,17 +2824,17 @@
       </c>
       <c r="AA3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5</v>
+        <v>3.3</v>
       </c>
       <c r="AB3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1</v>
+        <v>4.2</v>
       </c>
       <c r="AC3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="AD3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="AE3" t="s">
         <v>129</v>
@@ -2850,57 +2853,57 @@
       </c>
       <c r="AJ3" s="30"/>
       <c r="AK3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="AL3">
         <f t="shared" ref="AL3:AV8" ca="1" si="1">ROUND(RAND()*5,1)</f>
-        <v>0.9</v>
+        <v>2</v>
       </c>
       <c r="AM3">
         <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="AN3">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.5</v>
+      </c>
+      <c r="AO3">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.2</v>
+      </c>
+      <c r="AP3">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.9</v>
+      </c>
+      <c r="AQ3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="AR3">
+        <f t="shared" ca="1" si="1"/>
         <v>4.9000000000000004</v>
       </c>
-      <c r="AN3">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.6</v>
-      </c>
-      <c r="AO3">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.8</v>
-      </c>
-      <c r="AP3">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.5</v>
-      </c>
-      <c r="AQ3">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.4</v>
-      </c>
-      <c r="AR3">
+      <c r="AS3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="AT3">
         <f t="shared" ca="1" si="1"/>
         <v>2.4</v>
       </c>
-      <c r="AS3">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.1</v>
-      </c>
-      <c r="AT3">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.3</v>
-      </c>
       <c r="AU3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.6</v>
+        <v>0.5</v>
       </c>
       <c r="AV3">
         <f t="shared" ca="1" si="1"/>
         <v>2.9</v>
       </c>
       <c r="AW3" s="37" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="AX3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="AY3" s="21" t="s">
         <v>59</v>
@@ -2932,13 +2935,13 @@
         <v>46</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>143</v>
+        <v>166</v>
       </c>
       <c r="I4" s="19" t="s">
         <v>80</v>
       </c>
       <c r="J4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K4" t="s">
         <v>113</v>
@@ -2963,53 +2966,53 @@
       </c>
       <c r="R4" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>1.7</v>
+        <v>0.2</v>
       </c>
       <c r="S4" s="28">
         <f t="shared" ref="S4:S10" ca="1" si="2">ROUND(RAND()*5,1)</f>
-        <v>4</v>
+        <v>1.7</v>
       </c>
       <c r="T4" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>3.3</v>
+      </c>
+      <c r="U4" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.8</v>
+      </c>
+      <c r="V4" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.4</v>
+      </c>
+      <c r="W4" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>2.2000000000000002</v>
       </c>
-      <c r="U4" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="V4" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.7</v>
-      </c>
-      <c r="W4" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.6</v>
-      </c>
       <c r="X4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7</v>
+        <v>1.7</v>
       </c>
       <c r="Y4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4</v>
+        <v>3.6</v>
       </c>
       <c r="Z4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4</v>
+        <v>3.9</v>
       </c>
       <c r="AA4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4000000000000004</v>
+        <v>1.8</v>
       </c>
       <c r="AB4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4000000000000004</v>
+        <v>2.4</v>
       </c>
       <c r="AC4" s="28" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="AD4" s="28" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="AE4" t="s">
         <v>131</v>
@@ -3018,64 +3021,64 @@
         <v>1122334455</v>
       </c>
       <c r="AG4" s="28" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="AI4">
         <v>3224445566</v>
       </c>
       <c r="AJ4" s="30"/>
       <c r="AK4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="AL4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5</v>
+        <v>3.4</v>
       </c>
       <c r="AM4">
         <f t="shared" ca="1" si="1"/>
-        <v>3.6</v>
+        <v>1.2</v>
       </c>
       <c r="AN4">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7</v>
+        <v>4.5</v>
       </c>
       <c r="AO4">
         <f t="shared" ca="1" si="1"/>
-        <v>1.3</v>
+        <v>3.8</v>
       </c>
       <c r="AP4">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9</v>
+        <v>3.3</v>
       </c>
       <c r="AQ4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
       <c r="AR4">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AS4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.6</v>
+        <v>0.6</v>
       </c>
       <c r="AT4">
         <f t="shared" ca="1" si="1"/>
-        <v>4.2</v>
+        <v>3.5</v>
       </c>
       <c r="AU4">
         <f t="shared" ca="1" si="1"/>
-        <v>4.4000000000000004</v>
+        <v>1.2</v>
       </c>
       <c r="AV4">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9</v>
+        <v>4.3</v>
       </c>
       <c r="AW4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="AX4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="AY4" s="7" t="s">
         <v>57</v>
@@ -3092,7 +3095,7 @@
         <v>94</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>95</v>
@@ -3104,16 +3107,16 @@
         <v>69</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>143</v>
+        <v>166</v>
       </c>
       <c r="I5" s="19" t="s">
         <v>81</v>
       </c>
       <c r="J5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="K5" t="s">
         <v>114</v>
@@ -3134,57 +3137,57 @@
         <v>123</v>
       </c>
       <c r="Q5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R5" s="28">
         <f t="shared" ref="R5:R10" ca="1" si="3">ROUND(RAND()*5,1)</f>
-        <v>2.1</v>
+        <v>0.4</v>
       </c>
       <c r="S5" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>0.2</v>
+        <v>2.4</v>
       </c>
       <c r="T5" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>4.2</v>
+      </c>
+      <c r="U5" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="V5" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.6</v>
+      </c>
+      <c r="W5" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.8</v>
+      </c>
+      <c r="X5" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="U5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.9</v>
-      </c>
-      <c r="V5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.4</v>
-      </c>
-      <c r="W5" s="28">
+      <c r="Y5" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Z5" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AA5" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="AB5" s="28">
         <f t="shared" ca="1" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="X5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.5</v>
-      </c>
-      <c r="Y5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.7</v>
-      </c>
-      <c r="Z5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="AA5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.7</v>
-      </c>
-      <c r="AB5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.9000000000000004</v>
-      </c>
       <c r="AC5" s="28" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="AD5" s="28" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AE5" t="s">
         <v>132</v>
@@ -3193,7 +3196,7 @@
         <v>1234567890</v>
       </c>
       <c r="AG5" s="28" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="AH5">
         <v>3007778899</v>
@@ -3202,39 +3205,39 @@
         <v>3129991122</v>
       </c>
       <c r="AK5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="AL5">
         <f t="shared" ca="1" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="AM5">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="AN5">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.4</v>
+      </c>
+      <c r="AO5">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="AP5">
+        <f t="shared" ca="1" si="1"/>
         <v>4.4000000000000004</v>
       </c>
-      <c r="AM5">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AN5">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.6</v>
-      </c>
-      <c r="AO5">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="AP5">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.2</v>
-      </c>
       <c r="AQ5">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6</v>
+        <v>0.8</v>
       </c>
       <c r="AR5">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1</v>
+        <v>0.8</v>
       </c>
       <c r="AS5">
         <f t="shared" ca="1" si="1"/>
-        <v>3.9</v>
+        <v>1.4</v>
       </c>
       <c r="AT5">
         <f t="shared" ca="1" si="1"/>
@@ -3242,17 +3245,17 @@
       </c>
       <c r="AU5">
         <f t="shared" ca="1" si="1"/>
-        <v>3.1</v>
+        <v>4.2</v>
       </c>
       <c r="AV5">
         <f t="shared" ca="1" si="1"/>
-        <v>1.3</v>
+        <v>1.9</v>
       </c>
       <c r="AW5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="AX5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="AY5" s="21" t="s">
         <v>59</v>
@@ -3281,16 +3284,16 @@
         <v>75</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="I6" s="19" t="s">
         <v>82</v>
       </c>
       <c r="J6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K6" t="s">
         <v>115</v>
@@ -3311,57 +3314,57 @@
         <v>124</v>
       </c>
       <c r="Q6" s="17" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R6" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>4.8</v>
       </c>
       <c r="S6" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>2.2000000000000002</v>
+        <v>4.2</v>
       </c>
       <c r="T6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9</v>
+        <v>3.6</v>
       </c>
       <c r="U6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4.7</v>
       </c>
       <c r="V6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3</v>
+        <v>4.7</v>
       </c>
       <c r="W6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="X6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4</v>
+        <v>3.7</v>
       </c>
       <c r="Y6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7</v>
+        <v>3.4</v>
       </c>
       <c r="Z6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1000000000000001</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="AA6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6</v>
+        <v>2.1</v>
       </c>
       <c r="AB6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1</v>
+        <v>4</v>
       </c>
       <c r="AC6" s="28" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="AD6" s="28" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="AE6" t="s">
         <v>133</v>
@@ -3370,7 +3373,7 @@
         <v>1098765432</v>
       </c>
       <c r="AG6" s="28" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="AH6" s="17">
         <v>3173344556</v>
@@ -3380,57 +3383,57 @@
       </c>
       <c r="AJ6" s="17"/>
       <c r="AK6" s="17" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="AL6" s="18">
         <f t="shared" ca="1" si="1"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AM6" s="18">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="AN6" s="18">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.7</v>
+      </c>
+      <c r="AO6" s="18">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.7</v>
+      </c>
+      <c r="AP6" s="18">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="AQ6" s="18">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="AR6" s="18">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="AS6" s="18">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.7</v>
+      </c>
+      <c r="AT6" s="18">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.6</v>
+      </c>
+      <c r="AU6" s="18">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="AV6" s="18">
+        <f t="shared" ca="1" si="1"/>
         <v>0.7</v>
       </c>
-      <c r="AM6" s="18">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.6</v>
-      </c>
-      <c r="AN6" s="18">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.6</v>
-      </c>
-      <c r="AO6" s="18">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="AP6" s="18">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.7</v>
-      </c>
-      <c r="AQ6" s="18">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.8</v>
-      </c>
-      <c r="AR6" s="18">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.6</v>
-      </c>
-      <c r="AS6" s="18">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.9</v>
-      </c>
-      <c r="AT6" s="18">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.5</v>
-      </c>
-      <c r="AU6" s="18">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="AV6" s="18">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.8</v>
-      </c>
       <c r="AW6" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="AX6" s="18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AY6" s="7" t="s">
         <v>57</v>
@@ -3462,13 +3465,13 @@
         <v>46</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="I7" s="19" t="s">
         <v>83</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K7" t="s">
         <v>116</v>
@@ -3493,53 +3496,53 @@
       </c>
       <c r="R7" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="S7" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>2.8</v>
+        <v>2.7</v>
       </c>
       <c r="T7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>0.2</v>
       </c>
       <c r="U7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2999999999999998</v>
+        <v>0.9</v>
       </c>
       <c r="V7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2</v>
+        <v>0.4</v>
       </c>
       <c r="W7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="X7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5</v>
+        <v>2.1</v>
       </c>
       <c r="Y7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="Z7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4</v>
+        <v>1.9</v>
       </c>
       <c r="AA7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4</v>
+        <v>2.6</v>
       </c>
       <c r="AB7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="AC7" s="28" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="AD7" s="28" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="AE7" t="s">
         <v>134</v>
@@ -3548,7 +3551,7 @@
         <v>1000939523</v>
       </c>
       <c r="AG7" s="28" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="AH7">
         <v>3216677889</v>
@@ -3557,57 +3560,57 @@
         <v>3184455667</v>
       </c>
       <c r="AK7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="AL7">
         <f t="shared" ca="1" si="1"/>
-        <v>4.2</v>
+        <v>0.5</v>
       </c>
       <c r="AM7">
         <f t="shared" ca="1" si="1"/>
-        <v>4.3</v>
+        <v>3.7</v>
       </c>
       <c r="AN7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.1</v>
+        <v>1.3</v>
       </c>
       <c r="AO7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.5</v>
+        <v>1.6</v>
       </c>
       <c r="AP7">
         <f t="shared" ca="1" si="1"/>
-        <v>3.2</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="AQ7">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2</v>
+        <v>4.8</v>
       </c>
       <c r="AR7">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5</v>
+        <v>1</v>
       </c>
       <c r="AS7">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2</v>
+        <v>0.8</v>
       </c>
       <c r="AT7">
         <f t="shared" ca="1" si="1"/>
-        <v>4.0999999999999996</v>
+        <v>2.4</v>
       </c>
       <c r="AU7">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9</v>
+        <v>1.7</v>
       </c>
       <c r="AV7">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2.1</v>
       </c>
       <c r="AW7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="AX7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="AY7" s="7" t="s">
         <v>57</v>
@@ -3636,16 +3639,16 @@
         <v>69</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="I8" s="19" t="s">
         <v>84</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K8" t="s">
         <v>117</v>
@@ -3666,57 +3669,57 @@
         <v>126</v>
       </c>
       <c r="Q8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R8" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>0.1</v>
+        <v>3.7</v>
       </c>
       <c r="S8" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>2.2000000000000002</v>
+        <v>3.5</v>
       </c>
       <c r="T8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5</v>
+        <v>0.1</v>
       </c>
       <c r="U8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8</v>
+        <v>3.9</v>
       </c>
       <c r="V8" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="W8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.3</v>
+      </c>
+      <c r="X8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="Y8" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>1.8</v>
       </c>
-      <c r="W8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.4</v>
-      </c>
-      <c r="X8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="Y8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.4</v>
-      </c>
       <c r="Z8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8</v>
+        <v>0.9</v>
       </c>
       <c r="AA8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="AB8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4</v>
+        <v>4.2</v>
       </c>
       <c r="AC8" s="28" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="AD8" s="28" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="AE8" t="s">
         <v>135</v>
@@ -3734,57 +3737,57 @@
         <v>3248899001</v>
       </c>
       <c r="AK8" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="AL8">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="AM8">
         <f t="shared" ca="1" si="1"/>
-        <v>3.4</v>
+        <v>0.7</v>
       </c>
       <c r="AN8">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4</v>
+        <v>1.9</v>
       </c>
       <c r="AO8">
         <f t="shared" ca="1" si="1"/>
-        <v>3.8</v>
+        <v>2.8</v>
       </c>
       <c r="AP8">
         <f t="shared" ca="1" si="1"/>
-        <v>4.8</v>
+        <v>0.8</v>
       </c>
       <c r="AQ8">
         <f t="shared" ca="1" si="1"/>
-        <v>4.8</v>
+        <v>1.8</v>
       </c>
       <c r="AR8">
         <f t="shared" ca="1" si="1"/>
-        <v>4.7</v>
+        <v>1</v>
       </c>
       <c r="AS8">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1</v>
+        <v>4</v>
       </c>
       <c r="AT8">
         <f t="shared" ca="1" si="1"/>
-        <v>3.2</v>
+        <v>1.7</v>
       </c>
       <c r="AU8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="AV8">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AW8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="AX8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AY8" s="15" t="s">
         <v>58</v>
@@ -3816,13 +3819,13 @@
         <v>46</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
       <c r="I9" s="19" t="s">
         <v>85</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="K9" t="s">
         <v>118</v>
@@ -3847,53 +3850,53 @@
       </c>
       <c r="R9" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="S9" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>0.6</v>
+        <v>3.3</v>
       </c>
       <c r="T9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>2.7</v>
       </c>
       <c r="U9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5</v>
+        <v>2.9</v>
       </c>
       <c r="V9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>1.7</v>
       </c>
       <c r="W9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5</v>
+        <v>0.3</v>
       </c>
       <c r="X9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4</v>
+        <v>5</v>
       </c>
       <c r="Y9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="Z9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1</v>
+        <v>1.5</v>
       </c>
       <c r="AA9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2999999999999998</v>
+        <v>1.7</v>
       </c>
       <c r="AB9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>3.4</v>
       </c>
       <c r="AC9" s="28" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="AD9" s="28" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="AY9" s="7"/>
     </row>
@@ -3917,16 +3920,16 @@
         <v>69</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="I10" s="19" t="s">
         <v>119</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>120</v>
@@ -3944,43 +3947,43 @@
         <v>128</v>
       </c>
       <c r="Q10" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R10" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>1.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="S10" s="28">
         <f t="shared" ca="1" si="2"/>
+        <v>1.3</v>
+      </c>
+      <c r="T10" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="U10" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="V10" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="W10" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="X10" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="Y10" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="T10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.9</v>
-      </c>
-      <c r="U10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.6</v>
-      </c>
-      <c r="V10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="W10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.3</v>
-      </c>
-      <c r="X10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="Y10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
       <c r="Z10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2</v>
+        <v>3.5</v>
       </c>
       <c r="AA10" s="28">
         <f t="shared" ca="1" si="0"/>
@@ -3988,13 +3991,13 @@
       </c>
       <c r="AB10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7</v>
+        <v>0.2</v>
       </c>
       <c r="AC10" s="28" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="AD10" s="28" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="AY10" s="7"/>
     </row>
@@ -4021,13 +4024,13 @@
         <v>46</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="I11" s="19" t="s">
         <v>56</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="K11" t="s">
         <v>86</v>
@@ -4084,10 +4087,10 @@
         <v>0</v>
       </c>
       <c r="AC11" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="AD11" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:52" x14ac:dyDescent="0.25">
@@ -5485,10 +5488,10 @@
         <v>14</v>
       </c>
       <c r="S1" s="36" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="T1" s="33" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -5545,10 +5548,10 @@
         <v>3.1</v>
       </c>
       <c r="S2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="T2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -5572,27 +5575,27 @@
       </c>
       <c r="H3" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>3.1</v>
+        <v>2.1</v>
       </c>
       <c r="I3" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>4.4000000000000004</v>
+        <v>3.1</v>
       </c>
       <c r="J3" s="28">
         <f t="shared" ref="J3:R10" ca="1" si="0">ROUND(RAND()*5,1)</f>
-        <v>2.8</v>
+        <v>5</v>
       </c>
       <c r="K3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="L3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2000000000000002</v>
+        <v>0.1</v>
       </c>
       <c r="M3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="N3" s="28">
         <f t="shared" ca="1" si="0"/>
@@ -5600,25 +5603,25 @@
       </c>
       <c r="O3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="P3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2999999999999998</v>
+        <v>3.2</v>
       </c>
       <c r="Q3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9000000000000004</v>
+        <v>2</v>
       </c>
       <c r="R3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
       </c>
       <c r="S3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="T3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -5642,53 +5645,53 @@
       </c>
       <c r="H4" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>1.7</v>
+        <v>3.4</v>
       </c>
       <c r="I4" s="28">
         <f t="shared" ref="I4:I10" ca="1" si="1">ROUND(RAND()*5,1)</f>
-        <v>0.1</v>
+        <v>2.1</v>
       </c>
       <c r="J4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2</v>
+        <v>3.7</v>
       </c>
       <c r="K4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9000000000000004</v>
+        <v>1.3</v>
       </c>
       <c r="L4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="M4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8</v>
+        <v>0.8</v>
       </c>
       <c r="N4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1</v>
+        <v>3.6</v>
       </c>
       <c r="O4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="P4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="Q4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2</v>
+        <v>3.2</v>
       </c>
       <c r="R4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0999999999999996</v>
+        <v>3.3</v>
       </c>
       <c r="S4" s="28" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="T4" s="28" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -5712,53 +5715,53 @@
       </c>
       <c r="H5" s="28">
         <f t="shared" ref="H5:H10" ca="1" si="2">ROUND(RAND()*5,1)</f>
-        <v>3</v>
+        <v>1.4</v>
       </c>
       <c r="I5" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="J5" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>3.3</v>
+      </c>
+      <c r="K5" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.7</v>
+      </c>
+      <c r="L5" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.6</v>
+      </c>
+      <c r="M5" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N5" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.8</v>
+      </c>
+      <c r="O5" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>2.1</v>
       </c>
-      <c r="K5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.2</v>
-      </c>
-      <c r="L5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.7</v>
-      </c>
-      <c r="M5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.7</v>
-      </c>
-      <c r="N5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.9</v>
-      </c>
-      <c r="O5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.2</v>
-      </c>
       <c r="P5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7</v>
+        <v>3.9</v>
       </c>
       <c r="Q5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="R5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="S5" s="28" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="T5" s="28" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -5783,53 +5786,53 @@
       <c r="G6" s="17"/>
       <c r="H6" s="28">
         <f t="shared" ca="1" si="2"/>
+        <v>4.2</v>
+      </c>
+      <c r="I6" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.7</v>
+      </c>
+      <c r="J6" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>4.4000000000000004</v>
       </c>
-      <c r="I6" s="28">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.5</v>
-      </c>
-      <c r="J6" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.1</v>
-      </c>
       <c r="K6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="L6" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M6" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>3.7</v>
       </c>
-      <c r="M6" s="28">
+      <c r="N6" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="O6" s="28">
         <f t="shared" ca="1" si="0"/>
         <v>3.7</v>
       </c>
-      <c r="N6" s="28">
+      <c r="P6" s="28">
         <f t="shared" ca="1" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="O6" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.6</v>
-      </c>
-      <c r="P6" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.3</v>
-      </c>
       <c r="Q6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.3</v>
+        <v>5</v>
       </c>
       <c r="R6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1</v>
+        <v>0.3</v>
       </c>
       <c r="S6" s="28" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="T6" s="28" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -5853,35 +5856,35 @@
       </c>
       <c r="H7" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="I7" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1</v>
+        <v>1.7</v>
       </c>
       <c r="J7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>3.9</v>
       </c>
       <c r="K7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1</v>
+        <v>0.1</v>
       </c>
       <c r="L7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.3</v>
+        <v>0.8</v>
       </c>
       <c r="M7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4</v>
+        <v>4.2</v>
       </c>
       <c r="N7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1</v>
+        <v>3.7</v>
       </c>
       <c r="O7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7</v>
+        <v>1.9</v>
       </c>
       <c r="P7" s="28">
         <f t="shared" ca="1" si="0"/>
@@ -5889,17 +5892,17 @@
       </c>
       <c r="Q7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6</v>
+        <v>3.4</v>
       </c>
       <c r="R7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6</v>
+        <v>3.2</v>
       </c>
       <c r="S7" s="28" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="T7" s="28" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -5923,53 +5926,53 @@
       </c>
       <c r="H8" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>1.9</v>
+        <v>3.8</v>
       </c>
       <c r="I8" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>2.8</v>
       </c>
       <c r="J8" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="L8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.1</v>
+      </c>
+      <c r="M8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="N8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.8</v>
+      </c>
+      <c r="O8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="P8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="Q8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.2</v>
+      </c>
+      <c r="R8" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>3.8</v>
       </c>
-      <c r="K8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.8</v>
-      </c>
-      <c r="L8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.8</v>
-      </c>
-      <c r="M8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.8</v>
-      </c>
-      <c r="N8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="O8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.3</v>
-      </c>
-      <c r="P8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.7</v>
-      </c>
-      <c r="Q8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.6</v>
-      </c>
-      <c r="R8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.4</v>
-      </c>
       <c r="S8" s="28" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="T8" s="28" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -5993,53 +5996,53 @@
       </c>
       <c r="H9" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>0.2</v>
+        <v>2.7</v>
       </c>
       <c r="I9" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1000000000000001</v>
+        <v>1.7</v>
       </c>
       <c r="J9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9000000000000004</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="K9" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L9" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.9</v>
+      </c>
+      <c r="M9" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="N9" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="O9" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.9</v>
+      </c>
+      <c r="P9" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.1</v>
+      </c>
+      <c r="Q9" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="R9" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>1.7</v>
       </c>
-      <c r="L9" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.8</v>
-      </c>
-      <c r="M9" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.9</v>
-      </c>
-      <c r="N9" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.7</v>
-      </c>
-      <c r="O9" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.7</v>
-      </c>
-      <c r="P9" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.2</v>
-      </c>
-      <c r="Q9" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="R9" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.6</v>
-      </c>
       <c r="S9" s="28" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="T9" s="28" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -6060,53 +6063,53 @@
       </c>
       <c r="H10" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>4.2</v>
+        <v>1.5</v>
       </c>
       <c r="I10" s="28">
         <f t="shared" ca="1" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="J10" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="K10" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>2.4</v>
       </c>
-      <c r="J10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.7</v>
-      </c>
-      <c r="K10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.7</v>
-      </c>
       <c r="L10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4</v>
+        <v>2.9</v>
       </c>
       <c r="M10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="N10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4</v>
+        <v>3.7</v>
       </c>
       <c r="O10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="P10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9</v>
+        <v>0.3</v>
       </c>
       <c r="Q10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="R10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2</v>
+        <v>3.9</v>
       </c>
       <c r="S10" s="28" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="T10" s="28" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -6165,10 +6168,10 @@
         <v>0</v>
       </c>
       <c r="S11" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="T11" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -6225,10 +6228,10 @@
         <v>3.2</v>
       </c>
       <c r="S12" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="T12" s="29" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -6246,51 +6249,51 @@
       </c>
       <c r="F13" s="30"/>
       <c r="H13">
-        <f t="shared" ref="H13:R17" ca="1" si="3">ROUND(RAND()*5,1)</f>
-        <v>0.4</v>
+        <f t="shared" ref="H13:R16" ca="1" si="3">ROUND(RAND()*5,1)</f>
+        <v>2.6</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="3"/>
-        <v>4.4000000000000004</v>
+        <v>0.3</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="3"/>
-        <v>3.7</v>
+        <v>2.5</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="3"/>
-        <v>0.3</v>
+        <v>2.1</v>
       </c>
       <c r="M13">
         <f t="shared" ca="1" si="3"/>
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="3"/>
-        <v>1.5</v>
+        <v>3.6</v>
       </c>
       <c r="O13">
         <f t="shared" ca="1" si="3"/>
-        <v>2.4</v>
+        <v>0.8</v>
       </c>
       <c r="P13">
         <f t="shared" ca="1" si="3"/>
-        <v>1.4</v>
+        <v>3</v>
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="3"/>
-        <v>4.5</v>
+        <v>3.8</v>
       </c>
       <c r="R13">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="S13" s="37" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -6309,50 +6312,50 @@
       <c r="F14" s="30"/>
       <c r="H14">
         <f t="shared" ca="1" si="3"/>
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="3"/>
-        <v>1.4</v>
+        <v>2.4</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="3"/>
-        <v>0.6</v>
+        <v>3.5</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="3"/>
-        <v>2.8</v>
+        <v>4.8</v>
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="3"/>
-        <v>2.7</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="M14">
         <f t="shared" ca="1" si="3"/>
-        <v>2.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2.6</v>
       </c>
       <c r="O14">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>0.9</v>
       </c>
       <c r="P14">
         <f t="shared" ca="1" si="3"/>
-        <v>4.3</v>
+        <v>2.4</v>
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="3"/>
-        <v>4.4000000000000004</v>
+        <v>3.7</v>
       </c>
       <c r="R14">
         <f t="shared" ca="1" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.3</v>
       </c>
       <c r="S14" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -6374,46 +6377,46 @@
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="3"/>
-        <v>3.4</v>
+        <v>2.6</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="3"/>
-        <v>1.3</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="3"/>
-        <v>3.6</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="3"/>
-        <v>4.9000000000000004</v>
+        <v>3.2</v>
       </c>
       <c r="M15">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>1.3</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="3"/>
-        <v>4.9000000000000004</v>
+        <v>1</v>
       </c>
       <c r="O15">
         <f t="shared" ca="1" si="3"/>
-        <v>4.5999999999999996</v>
+        <v>1.7</v>
       </c>
       <c r="P15">
         <f t="shared" ca="1" si="3"/>
-        <v>2.4</v>
+        <v>2.8</v>
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="3"/>
-        <v>1.7</v>
+        <v>4.8</v>
       </c>
       <c r="R15">
         <f t="shared" ca="1" si="3"/>
-        <v>2.2999999999999998</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="S15" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -6434,50 +6437,50 @@
       <c r="G16" s="17"/>
       <c r="H16" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>1.3</v>
+        <v>1.9</v>
       </c>
       <c r="I16" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5</v>
+        <v>2.6</v>
       </c>
       <c r="J16" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>1.9</v>
+        <v>3.3</v>
       </c>
       <c r="K16" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>2.4</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="L16" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>0.7</v>
+        <v>1.8</v>
       </c>
       <c r="M16" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N16" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5</v>
+        <v>1.8</v>
       </c>
       <c r="O16" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>4.5999999999999996</v>
+        <v>3.5</v>
       </c>
       <c r="P16" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>1.8</v>
+        <v>4</v>
       </c>
       <c r="Q16" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="R16" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>4.5</v>
+        <v>1.6</v>
       </c>
       <c r="S16" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="T16" s="18"/>
     </row>

</xml_diff>

<commit_message>
🧑‍🎓Generar los la estructura de los mensajes junto con las Apis
</commit_message>
<xml_diff>
--- a/recursos/EmparejamientoFINAL.xlsx
+++ b/recursos/EmparejamientoFINAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\Sistema-TuGestor\recursos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\OneDrive\Documents\7 semestre\Sistema-TuGestor\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44994990-2746-4FD1-9077-A5F8535FAD76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F509F03-4B6E-4B48-B986-523A8F555468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14640" windowHeight="16305" tabRatio="670" xr2:uid="{FD9F6918-DD5F-4EFB-A5DA-81B3D2DC95CD}"/>
+    <workbookView xWindow="5115" yWindow="3015" windowWidth="15375" windowHeight="7785" tabRatio="670" xr2:uid="{FD9F6918-DD5F-4EFB-A5DA-81B3D2DC95CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Emparejamiento" sheetId="1" r:id="rId1"/>
@@ -324,9 +324,6 @@
     <t>jecheverry@javeriana.edu.co</t>
   </si>
   <si>
-    <t>312 8314004</t>
-  </si>
-  <si>
     <t>24</t>
   </si>
   <si>
@@ -592,6 +589,9 @@
   </si>
   <si>
     <t>100 horas - 1 tutorado</t>
+  </si>
+  <si>
+    <t>3128314004</t>
   </si>
 </sst>
 </file>
@@ -2398,8 +2398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D120C5C-D1E3-40C4-B4D7-C7D7020D0451}">
   <dimension ref="A1:AZ57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2447,7 +2447,7 @@
         <v>23</v>
       </c>
       <c r="J1" s="31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K1" s="11" t="s">
         <v>24</v>
@@ -2504,10 +2504,10 @@
         <v>14</v>
       </c>
       <c r="AC1" s="32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AD1" s="33" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AE1" s="13" t="s">
         <v>45</v>
@@ -2564,10 +2564,10 @@
         <v>43</v>
       </c>
       <c r="AW1" s="32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AX1" s="33" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AY1" s="9" t="s">
         <v>44</v>
@@ -2599,13 +2599,13 @@
         <v>46</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I2" s="16">
         <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K2" s="17" t="s">
         <v>70</v>
@@ -2662,13 +2662,13 @@
         <v>3.1</v>
       </c>
       <c r="AC2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AD2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AE2" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AF2" s="18">
         <v>1010944104</v>
@@ -2686,7 +2686,7 @@
         <v>73</v>
       </c>
       <c r="AK2" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AL2" s="29">
         <v>2.2999999999999998</v>
@@ -2722,10 +2722,10 @@
         <v>3.2</v>
       </c>
       <c r="AW2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AX2" s="29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AY2" s="21" t="s">
         <v>59</v>
@@ -2745,7 +2745,7 @@
         <v>78</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>79</v>
+        <v>168</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>68</v>
@@ -2754,19 +2754,19 @@
         <v>69</v>
       </c>
       <c r="G3" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="J3" t="s">
         <v>144</v>
       </c>
-      <c r="H3" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="J3" t="s">
-        <v>145</v>
-      </c>
       <c r="K3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L3" s="6">
         <v>1037883695</v>
@@ -2781,10 +2781,10 @@
         <v>3113735209</v>
       </c>
       <c r="P3" s="30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R3" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
@@ -2792,52 +2792,52 @@
       </c>
       <c r="S3" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>3</v>
+        <v>3.6</v>
       </c>
       <c r="T3" s="28">
         <f t="shared" ref="T3:AB10" ca="1" si="0">ROUND(RAND()*5,1)</f>
+        <v>0.8</v>
+      </c>
+      <c r="U3" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.7</v>
+      </c>
+      <c r="V3" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.7</v>
+      </c>
+      <c r="W3" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.1</v>
+      </c>
+      <c r="X3" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>2.1</v>
       </c>
-      <c r="U3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.7</v>
-      </c>
-      <c r="W3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="X3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.8</v>
-      </c>
       <c r="Y3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="Z3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="AA3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3</v>
+        <v>2.1</v>
       </c>
       <c r="AB3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2</v>
+        <v>1.7</v>
       </c>
       <c r="AC3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AD3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AE3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AF3">
         <v>1023456789</v>
@@ -2853,57 +2853,57 @@
       </c>
       <c r="AJ3" s="30"/>
       <c r="AK3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AL3">
         <f t="shared" ref="AL3:AV8" ca="1" si="1">ROUND(RAND()*5,1)</f>
-        <v>2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AM3">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>1.6</v>
       </c>
       <c r="AN3">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5</v>
+        <v>1.7</v>
       </c>
       <c r="AO3">
         <f t="shared" ca="1" si="1"/>
-        <v>3.2</v>
+        <v>3.6</v>
       </c>
       <c r="AP3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9</v>
+        <v>1.2</v>
       </c>
       <c r="AQ3">
         <f t="shared" ca="1" si="1"/>
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="AR3">
         <f t="shared" ca="1" si="1"/>
-        <v>4.9000000000000004</v>
+        <v>0.7</v>
       </c>
       <c r="AS3">
         <f t="shared" ca="1" si="1"/>
-        <v>0.1</v>
+        <v>4.2</v>
       </c>
       <c r="AT3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4</v>
+        <v>0.8</v>
       </c>
       <c r="AU3">
         <f t="shared" ca="1" si="1"/>
-        <v>0.5</v>
+        <v>3.8</v>
       </c>
       <c r="AV3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9</v>
+        <v>4.3</v>
       </c>
       <c r="AW3" s="37" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AX3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AY3" s="21" t="s">
         <v>59</v>
@@ -2914,19 +2914,19 @@
     </row>
     <row r="4" spans="1:52" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="E4" s="7" t="s">
         <v>136</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>137</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>75</v>
@@ -2935,16 +2935,16 @@
         <v>46</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L4" s="6">
         <v>1040872361</v>
@@ -2959,126 +2959,126 @@
         <v>3146538937</v>
       </c>
       <c r="P4" s="30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q4" t="s">
         <v>46</v>
       </c>
       <c r="R4" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="S4" s="28">
         <f t="shared" ref="S4:S10" ca="1" si="2">ROUND(RAND()*5,1)</f>
-        <v>1.7</v>
+        <v>4</v>
       </c>
       <c r="T4" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>2.8</v>
+      </c>
+      <c r="U4" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.6</v>
+      </c>
+      <c r="V4" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.3</v>
+      </c>
+      <c r="W4" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.6</v>
+      </c>
+      <c r="X4" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="Y4" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Z4" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AA4" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="AB4" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="U4" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.8</v>
-      </c>
-      <c r="V4" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.4</v>
-      </c>
-      <c r="W4" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="X4" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.7</v>
-      </c>
-      <c r="Y4" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.6</v>
-      </c>
-      <c r="Z4" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.9</v>
-      </c>
-      <c r="AA4" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.8</v>
-      </c>
-      <c r="AB4" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.4</v>
-      </c>
       <c r="AC4" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AD4" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AE4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AF4">
         <v>1122334455</v>
       </c>
       <c r="AG4" s="28" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AI4">
         <v>3224445566</v>
       </c>
       <c r="AJ4" s="30"/>
       <c r="AK4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AL4">
         <f t="shared" ca="1" si="1"/>
-        <v>3.4</v>
+        <v>4.2</v>
       </c>
       <c r="AM4">
         <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.4</v>
+      </c>
+      <c r="AO4">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="AP4">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AQ4">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AR4">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.8</v>
+      </c>
+      <c r="AS4">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AT4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="AU4">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.7</v>
+      </c>
+      <c r="AV4">
+        <f t="shared" ca="1" si="1"/>
         <v>1.2</v>
       </c>
-      <c r="AN4">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.5</v>
-      </c>
-      <c r="AO4">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.8</v>
-      </c>
-      <c r="AP4">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.3</v>
-      </c>
-      <c r="AQ4">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.9</v>
-      </c>
-      <c r="AR4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="AS4">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.6</v>
-      </c>
-      <c r="AT4">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.5</v>
-      </c>
-      <c r="AU4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.2</v>
-      </c>
-      <c r="AV4">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.3</v>
-      </c>
       <c r="AW4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AX4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AY4" s="7" t="s">
         <v>57</v>
@@ -3089,16 +3089,16 @@
     </row>
     <row r="5" spans="1:52" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>142</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>68</v>
@@ -3107,19 +3107,19 @@
         <v>69</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L5">
         <v>1040334221</v>
@@ -3134,69 +3134,69 @@
         <v>3025791188</v>
       </c>
       <c r="P5" s="30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Q5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R5" s="28">
         <f t="shared" ref="R5:R10" ca="1" si="3">ROUND(RAND()*5,1)</f>
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="S5" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>2.4</v>
+        <v>2.8</v>
       </c>
       <c r="T5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2</v>
+        <v>1.3</v>
       </c>
       <c r="U5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4</v>
+        <v>3.8</v>
       </c>
       <c r="V5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6</v>
+        <v>1.2</v>
       </c>
       <c r="W5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8</v>
+        <v>4.5</v>
       </c>
       <c r="X5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="Y5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1000000000000001</v>
+        <v>3.2</v>
       </c>
       <c r="Z5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="AA5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4</v>
+        <v>1.8</v>
       </c>
       <c r="AB5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="AC5" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AD5" s="28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AE5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF5">
         <v>1234567890</v>
       </c>
       <c r="AG5" s="28" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AH5">
         <v>3007778899</v>
@@ -3205,57 +3205,57 @@
         <v>3129991122</v>
       </c>
       <c r="AK5" t="s">
+        <v>158</v>
+      </c>
+      <c r="AL5">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AM5">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="AN5">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.1</v>
+      </c>
+      <c r="AO5">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="AP5">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.2</v>
+      </c>
+      <c r="AQ5">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="AR5">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.1</v>
+      </c>
+      <c r="AS5">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="AT5">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="AU5">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="AV5">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>145</v>
+      </c>
+      <c r="AX5" t="s">
         <v>159</v>
-      </c>
-      <c r="AL5">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="AM5">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.5</v>
-      </c>
-      <c r="AN5">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.4</v>
-      </c>
-      <c r="AO5">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.5</v>
-      </c>
-      <c r="AP5">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="AQ5">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.8</v>
-      </c>
-      <c r="AR5">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.8</v>
-      </c>
-      <c r="AS5">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.4</v>
-      </c>
-      <c r="AT5">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.8</v>
-      </c>
-      <c r="AU5">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.2</v>
-      </c>
-      <c r="AV5">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.9</v>
-      </c>
-      <c r="AW5" t="s">
-        <v>146</v>
-      </c>
-      <c r="AX5" t="s">
-        <v>160</v>
       </c>
       <c r="AY5" s="21" t="s">
         <v>59</v>
@@ -3272,10 +3272,10 @@
         <v>61</v>
       </c>
       <c r="C6" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>97</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>68</v>
@@ -3284,25 +3284,25 @@
         <v>75</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L6" s="6">
         <v>1046716109</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N6">
         <v>3243098774</v>
@@ -3311,69 +3311,69 @@
         <v>3044155979</v>
       </c>
       <c r="P6" s="27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q6" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R6" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>4.8</v>
+        <v>3.3</v>
       </c>
       <c r="S6" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>4.2</v>
+        <v>3.7</v>
       </c>
       <c r="T6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6</v>
+        <v>2.7</v>
       </c>
       <c r="U6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7</v>
+        <v>0.2</v>
       </c>
       <c r="V6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7</v>
+        <v>1.2</v>
       </c>
       <c r="W6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="X6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="Y6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4</v>
+        <v>2.1</v>
       </c>
       <c r="Z6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9000000000000004</v>
+        <v>1.9</v>
       </c>
       <c r="AA6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="AB6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3.2</v>
       </c>
       <c r="AC6" s="28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AD6" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AE6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AF6" s="18">
         <v>1098765432</v>
       </c>
       <c r="AG6" s="28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AH6" s="17">
         <v>3173344556</v>
@@ -3383,57 +3383,57 @@
       </c>
       <c r="AJ6" s="17"/>
       <c r="AK6" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AL6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2000000000000002</v>
+        <v>3.4</v>
       </c>
       <c r="AM6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.9</v>
+        <v>2.7</v>
       </c>
       <c r="AN6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AO6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7</v>
+        <v>1.8</v>
       </c>
       <c r="AP6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>4.9000000000000004</v>
+        <v>3.3</v>
       </c>
       <c r="AQ6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8</v>
+        <v>2.9</v>
       </c>
       <c r="AR6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AS6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7</v>
+        <v>2</v>
       </c>
       <c r="AT6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="AU6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.9</v>
+        <v>3.3</v>
       </c>
       <c r="AV6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.7</v>
+        <v>2.6</v>
       </c>
       <c r="AW6" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AX6" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AY6" s="7" t="s">
         <v>57</v>
@@ -3444,19 +3444,19 @@
     </row>
     <row r="7" spans="1:52" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="C7" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="E7" s="7" t="s">
         <v>138</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>139</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>69</v>
@@ -3465,16 +3465,16 @@
         <v>46</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L7" s="6">
         <v>1020316404</v>
@@ -3489,69 +3489,69 @@
         <v>3105528456</v>
       </c>
       <c r="P7" s="30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Q7" t="s">
         <v>46</v>
       </c>
       <c r="R7" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>1.8</v>
+        <v>3.3</v>
       </c>
       <c r="S7" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>2.7</v>
+        <v>4</v>
       </c>
       <c r="T7" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>4.3</v>
+      </c>
+      <c r="U7" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="V7" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.4</v>
+      </c>
+      <c r="W7" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="X7" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="Y7" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="Z7" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="AA7" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AB7" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="U7" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.9</v>
-      </c>
-      <c r="V7" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="W7" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.6</v>
-      </c>
-      <c r="X7" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.1</v>
-      </c>
-      <c r="Y7" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="Z7" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.9</v>
-      </c>
-      <c r="AA7" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.6</v>
-      </c>
-      <c r="AB7" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.9000000000000004</v>
-      </c>
       <c r="AC7" s="28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AD7" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AE7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AF7">
         <v>1000939523</v>
       </c>
       <c r="AG7" s="28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AH7">
         <v>3216677889</v>
@@ -3560,57 +3560,57 @@
         <v>3184455667</v>
       </c>
       <c r="AK7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AL7">
         <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AM7">
+        <f t="shared" ca="1" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="AM7">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.7</v>
-      </c>
       <c r="AN7">
         <f t="shared" ca="1" si="1"/>
-        <v>1.3</v>
+        <v>0.6</v>
       </c>
       <c r="AO7">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6</v>
+        <v>0.7</v>
       </c>
       <c r="AP7">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5999999999999996</v>
+        <v>0.9</v>
       </c>
       <c r="AQ7">
         <f t="shared" ca="1" si="1"/>
-        <v>4.8</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="AR7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>1.9</v>
       </c>
       <c r="AS7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="AT7">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4</v>
+        <v>4.7</v>
       </c>
       <c r="AU7">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7</v>
+        <v>3.6</v>
       </c>
       <c r="AV7">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1</v>
+        <v>2.6</v>
       </c>
       <c r="AW7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AX7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AY7" s="7" t="s">
         <v>57</v>
@@ -3621,16 +3621,16 @@
     </row>
     <row r="8" spans="1:52" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="D8" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>68</v>
@@ -3639,25 +3639,25 @@
         <v>69</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I8" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L8" s="6">
         <v>1137725488</v>
       </c>
       <c r="M8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N8">
         <v>3294344455</v>
@@ -3666,69 +3666,69 @@
         <v>3284344455</v>
       </c>
       <c r="P8" s="30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R8" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>3.7</v>
+        <v>0.6</v>
       </c>
       <c r="S8" s="28">
         <f t="shared" ca="1" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="T8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="U8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="V8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="W8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="X8" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="T8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="U8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.9</v>
-      </c>
-      <c r="V8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="W8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.3</v>
-      </c>
-      <c r="X8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.1</v>
-      </c>
       <c r="Y8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8</v>
+        <v>3.2</v>
       </c>
       <c r="Z8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9</v>
+        <v>2.5</v>
       </c>
       <c r="AA8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="AB8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2</v>
+        <v>3.2</v>
       </c>
       <c r="AC8" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AD8" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AE8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AF8">
         <v>1928412412</v>
       </c>
       <c r="AG8" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AH8">
         <v>3237788990</v>
@@ -3737,57 +3737,57 @@
         <v>3248899001</v>
       </c>
       <c r="AK8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AL8">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5</v>
+        <v>3.3</v>
       </c>
       <c r="AM8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="AN8">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9</v>
+        <v>4.2</v>
       </c>
       <c r="AO8">
         <f t="shared" ca="1" si="1"/>
-        <v>2.8</v>
+        <v>1.2</v>
       </c>
       <c r="AP8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="AQ8">
         <f t="shared" ca="1" si="1"/>
-        <v>1.8</v>
+        <v>4.3</v>
       </c>
       <c r="AR8">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2.4</v>
       </c>
       <c r="AS8">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AT8">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7</v>
+        <v>0.1</v>
       </c>
       <c r="AU8">
         <f t="shared" ca="1" si="1"/>
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
       <c r="AV8">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>3.7</v>
       </c>
       <c r="AW8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AX8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AY8" s="15" t="s">
         <v>58</v>
@@ -3798,19 +3798,19 @@
     </row>
     <row r="9" spans="1:52" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="E9" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>69</v>
@@ -3819,22 +3819,22 @@
         <v>46</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L9" s="6">
         <v>1070753987</v>
       </c>
       <c r="M9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N9">
         <v>3262122233</v>
@@ -3843,75 +3843,75 @@
         <v>3295455566</v>
       </c>
       <c r="P9" s="30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q9" t="s">
         <v>46</v>
       </c>
       <c r="R9" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>1.4</v>
+        <v>4</v>
       </c>
       <c r="S9" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>3.3</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="T9" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>3.4</v>
+      </c>
+      <c r="U9" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="V9" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.8</v>
+      </c>
+      <c r="W9" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>2.7</v>
       </c>
-      <c r="U9" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.9</v>
-      </c>
-      <c r="V9" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.7</v>
-      </c>
-      <c r="W9" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.3</v>
-      </c>
       <c r="X9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Y9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2000000000000002</v>
+        <v>4.3</v>
       </c>
       <c r="Z9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5</v>
+        <v>3.2</v>
       </c>
       <c r="AA9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="AB9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="AC9" s="28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AD9" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AY9" s="7"/>
     </row>
     <row r="10" spans="1:52" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="D10" s="7" t="s">
         <v>110</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>111</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>68</v>
@@ -3920,19 +3920,19 @@
         <v>69</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I10" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="K10" s="7" t="s">
         <v>119</v>
-      </c>
-      <c r="J10" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>120</v>
       </c>
       <c r="L10" s="6">
         <v>1070653287</v>
@@ -3944,60 +3944,60 @@
         <v>3251011123</v>
       </c>
       <c r="P10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Q10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R10" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>4.4000000000000004</v>
+        <v>3.4</v>
       </c>
       <c r="S10" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>1.3</v>
+        <v>4.3</v>
       </c>
       <c r="T10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7</v>
+        <v>3.3</v>
       </c>
       <c r="U10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="V10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="W10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2999999999999998</v>
+        <v>3</v>
       </c>
       <c r="X10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="Y10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="Z10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5</v>
+        <v>3.2</v>
       </c>
       <c r="AA10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2</v>
+        <v>4.2</v>
       </c>
       <c r="AB10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2</v>
+        <v>3.7</v>
       </c>
       <c r="AC10" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AD10" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AY10" s="7"/>
     </row>
@@ -4024,16 +4024,16 @@
         <v>46</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I11" s="19" t="s">
         <v>56</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L11" s="6">
         <v>1044655071</v>
@@ -4087,10 +4087,10 @@
         <v>0</v>
       </c>
       <c r="AC11" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AD11" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:52" x14ac:dyDescent="0.25">
@@ -5488,10 +5488,10 @@
         <v>14</v>
       </c>
       <c r="S1" s="36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T1" s="33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -5548,15 +5548,15 @@
         <v>3.1</v>
       </c>
       <c r="S2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="T2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B3" s="6">
         <v>1037883695</v>
@@ -5571,62 +5571,62 @@
         <v>3113735209</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H3" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>2.1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="I3" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>3.1</v>
+        <v>0.6</v>
       </c>
       <c r="J3" s="28">
         <f t="shared" ref="J3:R10" ca="1" si="0">ROUND(RAND()*5,1)</f>
-        <v>5</v>
+        <v>2.7</v>
       </c>
       <c r="K3" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="L3" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M3" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.1</v>
+      </c>
+      <c r="N3" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.7</v>
+      </c>
+      <c r="O3" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.1</v>
+      </c>
+      <c r="P3" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="Q3" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.3</v>
+      </c>
+      <c r="R3" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="L3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="M3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="N3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.1</v>
-      </c>
-      <c r="O3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="P3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.2</v>
-      </c>
-      <c r="Q3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="R3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.4</v>
-      </c>
       <c r="S3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B4" s="6">
         <v>1040872361</v>
@@ -5641,62 +5641,62 @@
         <v>3146538937</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H4" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>3.4</v>
+        <v>0.8</v>
       </c>
       <c r="I4" s="28">
         <f t="shared" ref="I4:I10" ca="1" si="1">ROUND(RAND()*5,1)</f>
-        <v>2.1</v>
+        <v>4</v>
       </c>
       <c r="J4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7</v>
+        <v>1.7</v>
       </c>
       <c r="K4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3</v>
+        <v>3.8</v>
       </c>
       <c r="L4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5</v>
+        <v>1.7</v>
       </c>
       <c r="M4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="N4" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>1.6</v>
+      </c>
+      <c r="O4" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.8</v>
+      </c>
+      <c r="P4" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="Q4" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="R4" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>3.6</v>
       </c>
-      <c r="O4" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="P4" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.4</v>
-      </c>
-      <c r="Q4" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.2</v>
-      </c>
-      <c r="R4" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.3</v>
-      </c>
       <c r="S4" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T4" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5">
         <v>1040334221</v>
@@ -5711,23 +5711,23 @@
         <v>3025791188</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H5" s="28">
         <f t="shared" ref="H5:H10" ca="1" si="2">ROUND(RAND()*5,1)</f>
-        <v>1.4</v>
+        <v>4.2</v>
       </c>
       <c r="I5" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="J5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3</v>
+        <v>0.6</v>
       </c>
       <c r="K5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7</v>
+        <v>3.8</v>
       </c>
       <c r="L5" s="28">
         <f t="shared" ca="1" si="0"/>
@@ -5735,44 +5735,44 @@
       </c>
       <c r="M5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0999999999999996</v>
+        <v>0.9</v>
       </c>
       <c r="N5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8</v>
+        <v>4.3</v>
       </c>
       <c r="O5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1</v>
+        <v>3.4</v>
       </c>
       <c r="P5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9</v>
+        <v>0.1</v>
       </c>
       <c r="Q5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="R5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9000000000000004</v>
+        <v>0.3</v>
       </c>
       <c r="S5" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="T5" s="28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B6" s="6">
         <v>1046716109</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D6">
         <v>3243098774</v>
@@ -5781,63 +5781,63 @@
         <v>3044155979</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G6" s="17"/>
       <c r="H6" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>4.2</v>
+        <v>2.1</v>
       </c>
       <c r="I6" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>4.7</v>
+        <v>3.6</v>
       </c>
       <c r="J6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4000000000000004</v>
+        <v>3.1</v>
       </c>
       <c r="K6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6</v>
+        <v>3.9</v>
       </c>
       <c r="L6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7</v>
+        <v>3.1</v>
       </c>
       <c r="N6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="O6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="P6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="Q6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2.9</v>
       </c>
       <c r="R6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3</v>
+        <v>1.8</v>
       </c>
       <c r="S6" s="28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="T6" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B7" s="6">
         <v>1020316404</v>
@@ -5852,68 +5852,68 @@
         <v>3105528456</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H7" s="28">
         <f t="shared" ca="1" si="2"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I7" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.3</v>
+      </c>
+      <c r="J7" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="K7" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.7</v>
+      </c>
+      <c r="L7" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="M7" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
-      <c r="I7" s="28">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.7</v>
-      </c>
-      <c r="J7" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.9</v>
-      </c>
-      <c r="K7" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="L7" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.8</v>
-      </c>
-      <c r="M7" s="28">
+      <c r="N7" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="O7" s="28">
         <f t="shared" ca="1" si="0"/>
         <v>4.2</v>
       </c>
-      <c r="N7" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.7</v>
-      </c>
-      <c r="O7" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.9</v>
-      </c>
       <c r="P7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9</v>
+        <v>2.8</v>
       </c>
       <c r="Q7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="R7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2</v>
+        <v>3.5</v>
       </c>
       <c r="S7" s="28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="T7" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B8" s="6">
         <v>1137725488</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D8">
         <v>3294344455</v>
@@ -5922,68 +5922,68 @@
         <v>3284344455</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H8" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>3.8</v>
+        <v>2.4</v>
       </c>
       <c r="I8" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>2.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="K8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0999999999999996</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="L8" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>1.8</v>
+      </c>
+      <c r="M8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.3</v>
+      </c>
+      <c r="N8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="O8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="P8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.4</v>
+      </c>
+      <c r="Q8" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>3.1</v>
       </c>
-      <c r="M8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="N8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.8</v>
-      </c>
-      <c r="O8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="P8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="Q8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.2</v>
-      </c>
       <c r="R8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8</v>
+        <v>2</v>
       </c>
       <c r="S8" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T8" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B9" s="6">
         <v>1070753987</v>
       </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D9">
         <v>3262122233</v>
@@ -5992,62 +5992,62 @@
         <v>3295455566</v>
       </c>
       <c r="F9" s="30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H9" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>2.7</v>
+        <v>1.3</v>
       </c>
       <c r="I9" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7</v>
+        <v>2.4</v>
       </c>
       <c r="J9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="K9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>0.8</v>
       </c>
       <c r="L9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9</v>
+        <v>3.1</v>
       </c>
       <c r="M9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8</v>
+        <v>1.3</v>
       </c>
       <c r="N9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4</v>
+        <v>4.7</v>
       </c>
       <c r="O9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9</v>
+        <v>4</v>
       </c>
       <c r="P9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1</v>
+        <v>3.7</v>
       </c>
       <c r="Q9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5</v>
+        <v>2.8</v>
       </c>
       <c r="R9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7</v>
+        <v>1.4</v>
       </c>
       <c r="S9" s="28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="T9" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B10" s="6">
         <v>1070653287</v>
@@ -6059,62 +6059,62 @@
         <v>3251011123</v>
       </c>
       <c r="F10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H10" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>1.5</v>
+        <v>4.8</v>
       </c>
       <c r="I10" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.4</v>
+        <v>4.2</v>
       </c>
       <c r="J10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5</v>
+        <v>3.1</v>
       </c>
       <c r="K10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4</v>
+        <v>1.3</v>
       </c>
       <c r="L10" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>4.7</v>
+      </c>
+      <c r="M10" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>2.9</v>
       </c>
-      <c r="M10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
       <c r="N10" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>2.8</v>
+      </c>
+      <c r="O10" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="P10" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>3.7</v>
       </c>
-      <c r="O10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="P10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.3</v>
-      </c>
       <c r="Q10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2000000000000002</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="R10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9</v>
+        <v>3.4</v>
       </c>
       <c r="S10" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T10" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B11" s="6">
         <v>1044655071</v>
@@ -6168,15 +6168,15 @@
         <v>0</v>
       </c>
       <c r="S11" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="T11" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B12" s="18">
         <v>1010944104</v>
@@ -6228,15 +6228,15 @@
         <v>3.2</v>
       </c>
       <c r="S12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T12" s="29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B13">
         <v>1023456789</v>
@@ -6250,55 +6250,55 @@
       <c r="F13" s="30"/>
       <c r="H13">
         <f t="shared" ref="H13:R16" ca="1" si="3">ROUND(RAND()*5,1)</f>
-        <v>2.6</v>
+        <v>4.5</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="3"/>
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="3"/>
-        <v>2.5</v>
+        <v>3.6</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="3"/>
-        <v>3.8</v>
+        <v>1.3</v>
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="3"/>
-        <v>2.1</v>
+        <v>3.6</v>
       </c>
       <c r="M13">
         <f t="shared" ca="1" si="3"/>
-        <v>4.9000000000000004</v>
+        <v>4</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="3"/>
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
       <c r="O13">
         <f t="shared" ca="1" si="3"/>
-        <v>0.8</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="P13">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="3"/>
-        <v>3.8</v>
+        <v>0.2</v>
       </c>
       <c r="R13">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="S13" s="37" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B14">
         <v>1122334455</v>
@@ -6312,39 +6312,39 @@
       <c r="F14" s="30"/>
       <c r="H14">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>2.1</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="3"/>
-        <v>2.4</v>
+        <v>0.8</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="3"/>
-        <v>4.8</v>
+        <v>2.9</v>
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="3"/>
-        <v>4.9000000000000004</v>
+        <v>1.5</v>
       </c>
       <c r="M14">
         <f t="shared" ca="1" si="3"/>
-        <v>1.1000000000000001</v>
+        <v>2.5</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="3"/>
-        <v>2.6</v>
+        <v>1.6</v>
       </c>
       <c r="O14">
         <f t="shared" ca="1" si="3"/>
-        <v>0.9</v>
+        <v>1.5</v>
       </c>
       <c r="P14">
         <f t="shared" ca="1" si="3"/>
-        <v>2.4</v>
+        <v>1</v>
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="3"/>
@@ -6352,15 +6352,15 @@
       </c>
       <c r="R14">
         <f t="shared" ca="1" si="3"/>
-        <v>3.3</v>
+        <v>3</v>
       </c>
       <c r="S14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B15">
         <v>1234567890</v>
@@ -6373,55 +6373,55 @@
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="3"/>
-        <v>0.6</v>
+        <v>4.8</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="3"/>
-        <v>2.6</v>
+        <v>4.8</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="3"/>
-        <v>4.0999999999999996</v>
+        <v>4.8</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="3"/>
-        <v>4.9000000000000004</v>
+        <v>2.9</v>
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="3"/>
-        <v>3.2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="M15">
         <f t="shared" ca="1" si="3"/>
-        <v>1.3</v>
+        <v>3.6</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="O15">
         <f t="shared" ca="1" si="3"/>
-        <v>1.7</v>
+        <v>2.7</v>
       </c>
       <c r="P15">
         <f t="shared" ca="1" si="3"/>
-        <v>2.8</v>
+        <v>3.2</v>
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="3"/>
-        <v>4.8</v>
+        <v>0.2</v>
       </c>
       <c r="R15">
         <f t="shared" ca="1" si="3"/>
-        <v>4.4000000000000004</v>
+        <v>3.6</v>
       </c>
       <c r="S15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B16" s="18">
         <v>1098765432</v>
@@ -6437,50 +6437,50 @@
       <c r="G16" s="17"/>
       <c r="H16" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>1.9</v>
+        <v>3.2</v>
       </c>
       <c r="I16" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>2.6</v>
+        <v>0.1</v>
       </c>
       <c r="J16" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>3.3</v>
+        <v>5</v>
       </c>
       <c r="K16" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>1.1000000000000001</v>
+        <v>3.8</v>
       </c>
       <c r="L16" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>1.8</v>
+        <v>2.9</v>
       </c>
       <c r="M16" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3.1</v>
       </c>
       <c r="N16" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
       <c r="O16" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="P16" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="Q16" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>1.5</v>
+        <v>3.8</v>
       </c>
       <c r="R16" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
       <c r="S16" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T16" s="18"/>
     </row>

</xml_diff>

<commit_message>
🎞️Correcion del json y monitoreo
</commit_message>
<xml_diff>
--- a/recursos/EmparejamientoFINAL.xlsx
+++ b/recursos/EmparejamientoFINAL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\OneDrive\Documents\7 semestre\Sistema-TuGestor\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F509F03-4B6E-4B48-B986-523A8F555468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B36BCE5-7918-4734-9315-C24F8CF79723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="3015" windowWidth="15375" windowHeight="7785" tabRatio="670" xr2:uid="{FD9F6918-DD5F-4EFB-A5DA-81B3D2DC95CD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="670" xr2:uid="{FD9F6918-DD5F-4EFB-A5DA-81B3D2DC95CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Emparejamiento" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="176">
   <si>
     <t>1.id</t>
   </si>
@@ -592,6 +592,27 @@
   </si>
   <si>
     <t>3128314004</t>
+  </si>
+  <si>
+    <t>Colegio San Angelo</t>
+  </si>
+  <si>
+    <t>CorreoEjemplo323@gmail.com</t>
+  </si>
+  <si>
+    <t>CorreoEjemplo3333@gmail.com</t>
+  </si>
+  <si>
+    <t>CorreoEjemplo444@gmail.com</t>
+  </si>
+  <si>
+    <t>CorreoEjemplo555@gmail.com</t>
+  </si>
+  <si>
+    <t>CorreoEjemplo666@gmail.com</t>
+  </si>
+  <si>
+    <t>CorreoEjemplo777@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -966,26 +987,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1046,6 +1047,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1056,6 +1077,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1066,21 +1097,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1106,6 +1127,226 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1136,6 +1377,106 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1156,146 +1497,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1336,6 +1537,126 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1346,96 +1667,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1446,6 +1677,86 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1456,6 +1767,156 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1481,446 +1942,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2398,8 +2419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D120C5C-D1E3-40C4-B4D7-C7D7020D0451}">
   <dimension ref="A1:AZ57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2788,47 +2809,47 @@
       </c>
       <c r="R3" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>3.4</v>
+        <v>3.9</v>
       </c>
       <c r="S3" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>3.6</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="T3" s="28">
         <f t="shared" ref="T3:AB10" ca="1" si="0">ROUND(RAND()*5,1)</f>
+        <v>0.9</v>
+      </c>
+      <c r="U3" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="V3" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="W3" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="X3" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.7</v>
+      </c>
+      <c r="Y3" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.6</v>
+      </c>
+      <c r="Z3" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AA3" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="U3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.7</v>
-      </c>
-      <c r="V3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.7</v>
-      </c>
-      <c r="W3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.1</v>
-      </c>
-      <c r="X3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.1</v>
-      </c>
-      <c r="Y3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="Z3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="AA3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.1</v>
-      </c>
       <c r="AB3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7</v>
+        <v>3.5</v>
       </c>
       <c r="AC3" t="s">
         <v>144</v>
@@ -2851,53 +2872,55 @@
       <c r="AI3">
         <v>3155551212</v>
       </c>
-      <c r="AJ3" s="30"/>
+      <c r="AJ3" s="27" t="s">
+        <v>170</v>
+      </c>
       <c r="AK3" t="s">
         <v>158</v>
       </c>
       <c r="AL3">
         <f t="shared" ref="AL3:AV8" ca="1" si="1">ROUND(RAND()*5,1)</f>
-        <v>1.1000000000000001</v>
+        <v>4.2</v>
       </c>
       <c r="AM3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6</v>
+        <v>4.8</v>
       </c>
       <c r="AN3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7</v>
+        <v>4</v>
       </c>
       <c r="AO3">
         <f t="shared" ca="1" si="1"/>
-        <v>3.6</v>
+        <v>0.1</v>
       </c>
       <c r="AP3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AQ3">
         <f t="shared" ca="1" si="1"/>
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="AR3">
         <f t="shared" ca="1" si="1"/>
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="AS3">
         <f t="shared" ca="1" si="1"/>
-        <v>4.2</v>
+        <v>1.3</v>
       </c>
       <c r="AT3">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AU3">
         <f t="shared" ca="1" si="1"/>
-        <v>3.8</v>
+        <v>1.3</v>
       </c>
       <c r="AV3">
         <f t="shared" ca="1" si="1"/>
-        <v>4.3</v>
+        <v>3.4</v>
       </c>
       <c r="AW3" s="37" t="s">
         <v>144</v>
@@ -2966,47 +2989,47 @@
       </c>
       <c r="R4" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>0.3</v>
+        <v>4.8</v>
       </c>
       <c r="S4" s="28">
         <f t="shared" ref="S4:S10" ca="1" si="2">ROUND(RAND()*5,1)</f>
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="T4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="U4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6</v>
+        <v>0.7</v>
       </c>
       <c r="V4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.3</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="W4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.6</v>
+        <v>2.1</v>
       </c>
       <c r="X4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="Y4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2000000000000002</v>
+        <v>1.5</v>
       </c>
       <c r="Z4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4000000000000004</v>
+        <v>0.1</v>
       </c>
       <c r="AA4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8</v>
+        <v>3.5</v>
       </c>
       <c r="AB4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3</v>
+        <v>1.6</v>
       </c>
       <c r="AC4" s="28" t="s">
         <v>153</v>
@@ -3023,56 +3046,61 @@
       <c r="AG4" s="28" t="s">
         <v>160</v>
       </c>
+      <c r="AH4">
+        <v>3112223344</v>
+      </c>
       <c r="AI4">
         <v>3224445566</v>
       </c>
-      <c r="AJ4" s="30"/>
+      <c r="AJ4" s="27" t="s">
+        <v>171</v>
+      </c>
       <c r="AK4" t="s">
         <v>157</v>
       </c>
       <c r="AL4">
         <f t="shared" ca="1" si="1"/>
-        <v>4.2</v>
+        <v>4.8</v>
       </c>
       <c r="AM4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4</v>
+        <v>2.8</v>
       </c>
       <c r="AO4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="AP4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2000000000000002</v>
+        <v>2.1</v>
       </c>
       <c r="AQ4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2000000000000002</v>
+        <v>3.7</v>
       </c>
       <c r="AR4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AS4">
         <f t="shared" ca="1" si="1"/>
-        <v>4.0999999999999996</v>
+        <v>3.5</v>
       </c>
       <c r="AT4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.9</v>
+        <v>2.4</v>
       </c>
       <c r="AU4">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7</v>
+        <v>1</v>
       </c>
       <c r="AV4">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="AW4" t="s">
         <v>147</v>
@@ -3141,47 +3169,47 @@
       </c>
       <c r="R5" s="28">
         <f t="shared" ref="R5:R10" ca="1" si="3">ROUND(RAND()*5,1)</f>
-        <v>0</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="S5" s="28">
         <f t="shared" ca="1" si="2"/>
+        <v>2.6</v>
+      </c>
+      <c r="T5" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="U5" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.7</v>
+      </c>
+      <c r="V5" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="W5" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="X5" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>2.8</v>
       </c>
-      <c r="T5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.3</v>
-      </c>
-      <c r="U5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.8</v>
-      </c>
-      <c r="V5" s="28">
+      <c r="Y5" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.6</v>
+      </c>
+      <c r="Z5" s="28">
         <f t="shared" ca="1" si="0"/>
         <v>1.2</v>
       </c>
-      <c r="W5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="X5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="Y5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.2</v>
-      </c>
-      <c r="Z5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.2000000000000002</v>
-      </c>
       <c r="AA5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8</v>
+        <v>1.2</v>
       </c>
       <c r="AB5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9</v>
+        <v>4.8</v>
       </c>
       <c r="AC5" s="28" t="s">
         <v>146</v>
@@ -3204,52 +3232,55 @@
       <c r="AI5">
         <v>3129991122</v>
       </c>
+      <c r="AJ5" s="27" t="s">
+        <v>172</v>
+      </c>
       <c r="AK5" t="s">
         <v>158</v>
       </c>
       <c r="AL5">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5999999999999996</v>
+        <v>4.8</v>
       </c>
       <c r="AM5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.7</v>
+        <v>1.6</v>
       </c>
       <c r="AN5">
         <f t="shared" ca="1" si="1"/>
-        <v>3.1</v>
+        <v>2.5</v>
       </c>
       <c r="AO5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2</v>
+        <v>2.6</v>
       </c>
       <c r="AP5">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2</v>
+        <v>0.1</v>
       </c>
       <c r="AQ5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.4</v>
+        <v>2.6</v>
       </c>
       <c r="AR5">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="AS5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.9</v>
+        <v>1.5</v>
       </c>
       <c r="AT5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.6</v>
+        <v>2.5</v>
       </c>
       <c r="AU5">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AV5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="AW5" t="s">
         <v>145</v>
@@ -3318,47 +3349,47 @@
       </c>
       <c r="R6" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>3.3</v>
+        <v>0.3</v>
       </c>
       <c r="S6" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>3.7</v>
+        <v>1.6</v>
       </c>
       <c r="T6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7</v>
+        <v>3.5</v>
       </c>
       <c r="U6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2</v>
+        <v>3.6</v>
       </c>
       <c r="V6" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>1.8</v>
+      </c>
+      <c r="W6" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.8</v>
+      </c>
+      <c r="X6" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>1.2</v>
       </c>
-      <c r="W6" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="X6" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.9000000000000004</v>
-      </c>
       <c r="Y6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1</v>
+        <v>0.9</v>
       </c>
       <c r="Z6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="AA6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2999999999999998</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="AB6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="AC6" s="28" t="s">
         <v>151</v>
@@ -3381,53 +3412,55 @@
       <c r="AI6" s="17">
         <v>3195566778</v>
       </c>
-      <c r="AJ6" s="17"/>
+      <c r="AJ6" s="27" t="s">
+        <v>173</v>
+      </c>
       <c r="AK6" s="17" t="s">
         <v>158</v>
       </c>
       <c r="AL6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>3.4</v>
+        <v>0.1</v>
       </c>
       <c r="AM6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7</v>
+        <v>4.3</v>
       </c>
       <c r="AN6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1000000000000001</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="AO6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>1.8</v>
+        <v>0.8</v>
       </c>
       <c r="AP6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>3.3</v>
+        <v>2.7</v>
       </c>
       <c r="AQ6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9</v>
+        <v>0.9</v>
       </c>
       <c r="AR6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="AS6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3.4</v>
       </c>
       <c r="AT6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>4.4000000000000004</v>
+        <v>4</v>
       </c>
       <c r="AU6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>3.3</v>
+        <v>0.2</v>
       </c>
       <c r="AV6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>2.6</v>
+        <v>3.1</v>
       </c>
       <c r="AW6" s="18" t="s">
         <v>152</v>
@@ -3496,47 +3529,47 @@
       </c>
       <c r="R7" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>3.3</v>
+        <v>2</v>
       </c>
       <c r="S7" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>0.7</v>
       </c>
       <c r="T7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.3</v>
+        <v>3.8</v>
       </c>
       <c r="U7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="V7" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="W7" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.7</v>
+      </c>
+      <c r="X7" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="Y7" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.4</v>
+      </c>
+      <c r="Z7" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>3.4</v>
       </c>
-      <c r="W7" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="X7" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.8</v>
-      </c>
-      <c r="Y7" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.3</v>
-      </c>
-      <c r="Z7" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.5</v>
-      </c>
       <c r="AA7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2000000000000002</v>
+        <v>1.7</v>
       </c>
       <c r="AB7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="AC7" s="28" t="s">
         <v>145</v>
@@ -3564,47 +3597,47 @@
       </c>
       <c r="AL7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AM7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.5</v>
+        <v>3.2</v>
       </c>
       <c r="AN7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.6</v>
+        <v>3.2</v>
       </c>
       <c r="AO7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.7</v>
+        <v>4.2</v>
       </c>
       <c r="AP7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.9</v>
+        <v>2.7</v>
       </c>
       <c r="AQ7">
         <f t="shared" ca="1" si="1"/>
-        <v>4.0999999999999996</v>
+        <v>1.2</v>
       </c>
       <c r="AR7">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9</v>
+        <v>1.2</v>
       </c>
       <c r="AS7">
         <f t="shared" ca="1" si="1"/>
-        <v>4.0999999999999996</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="AT7">
         <f t="shared" ca="1" si="1"/>
-        <v>4.7</v>
+        <v>4.8</v>
       </c>
       <c r="AU7">
         <f t="shared" ca="1" si="1"/>
-        <v>3.6</v>
+        <v>2.5</v>
       </c>
       <c r="AV7">
         <f t="shared" ca="1" si="1"/>
-        <v>2.6</v>
+        <v>3</v>
       </c>
       <c r="AW7" t="s">
         <v>144</v>
@@ -3673,47 +3706,47 @@
       </c>
       <c r="R8" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>0.6</v>
+        <v>2.8</v>
       </c>
       <c r="S8" s="28">
         <f t="shared" ca="1" si="2"/>
+        <v>3.4</v>
+      </c>
+      <c r="T8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.4</v>
+      </c>
+      <c r="U8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.7</v>
+      </c>
+      <c r="V8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.4</v>
+      </c>
+      <c r="W8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="X8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.9</v>
+      </c>
+      <c r="Y8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.9</v>
+      </c>
+      <c r="Z8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.4</v>
+      </c>
+      <c r="AA8" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="T8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.5</v>
-      </c>
-      <c r="U8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.8</v>
-      </c>
-      <c r="V8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="W8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.7</v>
-      </c>
-      <c r="X8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.5</v>
-      </c>
-      <c r="Y8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.2</v>
-      </c>
-      <c r="Z8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.5</v>
-      </c>
-      <c r="AA8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
       <c r="AB8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2</v>
+        <v>2.4</v>
       </c>
       <c r="AC8" s="28" t="s">
         <v>153</v>
@@ -3741,47 +3774,47 @@
       </c>
       <c r="AL8">
         <f t="shared" ca="1" si="1"/>
-        <v>3.3</v>
+        <v>3.7</v>
       </c>
       <c r="AM8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8</v>
+        <v>4</v>
       </c>
       <c r="AN8">
         <f t="shared" ca="1" si="1"/>
-        <v>4.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="AO8">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2</v>
+        <v>0.7</v>
       </c>
       <c r="AP8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.6</v>
+        <v>3.6</v>
       </c>
       <c r="AQ8">
         <f t="shared" ca="1" si="1"/>
-        <v>4.3</v>
+        <v>3.8</v>
       </c>
       <c r="AR8">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4</v>
+        <v>4.8</v>
       </c>
       <c r="AS8">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AT8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.1</v>
+        <v>1.7</v>
       </c>
       <c r="AU8">
         <f t="shared" ca="1" si="1"/>
-        <v>4.7</v>
+        <v>4</v>
       </c>
       <c r="AV8">
         <f t="shared" ca="1" si="1"/>
-        <v>3.7</v>
+        <v>0.3</v>
       </c>
       <c r="AW8" t="s">
         <v>152</v>
@@ -3850,47 +3883,47 @@
       </c>
       <c r="R9" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="S9" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>4.5999999999999996</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="T9" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>1.8</v>
+      </c>
+      <c r="U9" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>3.4</v>
       </c>
-      <c r="U9" s="28">
+      <c r="V9" s="28">
         <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
-      <c r="V9" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.8</v>
-      </c>
       <c r="W9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7</v>
+        <v>1.5</v>
       </c>
       <c r="X9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1000000000000001</v>
+        <v>4.7</v>
       </c>
       <c r="Y9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.3</v>
+        <v>0.5</v>
       </c>
       <c r="Z9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="AA9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4000000000000004</v>
+        <v>3.3</v>
       </c>
       <c r="AB9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6</v>
+        <v>0.2</v>
       </c>
       <c r="AC9" s="28" t="s">
         <v>145</v>
@@ -3937,6 +3970,9 @@
       <c r="L10" s="6">
         <v>1070653287</v>
       </c>
+      <c r="M10" t="s">
+        <v>169</v>
+      </c>
       <c r="N10">
         <v>3249900112</v>
       </c>
@@ -3951,47 +3987,47 @@
       </c>
       <c r="R10" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>3.4</v>
+        <v>1.2</v>
       </c>
       <c r="S10" s="28">
         <f t="shared" ca="1" si="2"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="T10" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="U10" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.9</v>
+      </c>
+      <c r="V10" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.6</v>
+      </c>
+      <c r="W10" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="X10" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="Y10" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.2</v>
+      </c>
+      <c r="Z10" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="AA10" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.7</v>
+      </c>
+      <c r="AB10" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>4.3</v>
-      </c>
-      <c r="T10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.3</v>
-      </c>
-      <c r="U10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="V10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.4</v>
-      </c>
-      <c r="W10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="X10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="Y10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="Z10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.2</v>
-      </c>
-      <c r="AA10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.2</v>
-      </c>
-      <c r="AB10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.7</v>
       </c>
       <c r="AC10" s="28" t="s">
         <v>153</v>
@@ -5289,25 +5325,25 @@
     <cfRule type="duplicateValues" dxfId="120" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:G1">
-    <cfRule type="duplicateValues" dxfId="119" priority="84"/>
-    <cfRule type="duplicateValues" dxfId="118" priority="77"/>
-    <cfRule type="duplicateValues" dxfId="117" priority="85"/>
-    <cfRule type="duplicateValues" dxfId="116" priority="76"/>
-    <cfRule type="duplicateValues" dxfId="115" priority="75"/>
-    <cfRule type="duplicateValues" dxfId="114" priority="74"/>
-    <cfRule type="duplicateValues" dxfId="113" priority="72"/>
-    <cfRule type="duplicateValues" dxfId="112" priority="73"/>
+    <cfRule type="duplicateValues" dxfId="119" priority="72"/>
+    <cfRule type="duplicateValues" dxfId="118" priority="73"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="74"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="75"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="76"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="77"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="84"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="85"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:L1">
-    <cfRule type="duplicateValues" dxfId="111" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="39"/>
     <cfRule type="duplicateValues" dxfId="110" priority="41"/>
-    <cfRule type="duplicateValues" dxfId="109" priority="53"/>
-    <cfRule type="duplicateValues" dxfId="108" priority="52"/>
-    <cfRule type="duplicateValues" dxfId="107" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="107" priority="44"/>
     <cfRule type="duplicateValues" dxfId="106" priority="48"/>
-    <cfRule type="duplicateValues" dxfId="105" priority="39"/>
-    <cfRule type="duplicateValues" dxfId="104" priority="44"/>
-    <cfRule type="duplicateValues" dxfId="103" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="105" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="104" priority="52"/>
+    <cfRule type="duplicateValues" dxfId="103" priority="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:L6">
     <cfRule type="duplicateValues" dxfId="102" priority="15"/>
@@ -5358,13 +5394,13 @@
     <cfRule type="duplicateValues" dxfId="87" priority="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE1:AF1">
-    <cfRule type="duplicateValues" dxfId="86" priority="40"/>
-    <cfRule type="duplicateValues" dxfId="85" priority="38"/>
-    <cfRule type="duplicateValues" dxfId="84" priority="46"/>
-    <cfRule type="duplicateValues" dxfId="83" priority="47"/>
-    <cfRule type="duplicateValues" dxfId="82" priority="54"/>
-    <cfRule type="duplicateValues" dxfId="81" priority="45"/>
-    <cfRule type="duplicateValues" dxfId="80" priority="51"/>
+    <cfRule type="duplicateValues" dxfId="86" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="85" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="84" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="83" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="82" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="81" priority="51"/>
+    <cfRule type="duplicateValues" dxfId="80" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE2:AF2 K7:L18 L5:M6 K3:L5">
     <cfRule type="duplicateValues" dxfId="79" priority="36"/>
@@ -5393,34 +5429,38 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{35CA5F4C-EC76-4BAF-A154-28FD229AB29C}"/>
     <hyperlink ref="P2" r:id="rId2" xr:uid="{5682C1AD-FB9D-4AAD-9720-D9FC3E06F2B7}"/>
-    <hyperlink ref="AJ2" r:id="rId3" xr:uid="{03626D1D-4287-4857-BF5D-A6A8D70EC51F}"/>
-    <hyperlink ref="C3" r:id="rId4" xr:uid="{1A0B751A-EE31-44F8-BE4B-F6918B4B56D5}"/>
-    <hyperlink ref="C4" r:id="rId5" xr:uid="{F706650C-E410-4E01-AB01-9A6E74B2CA2F}"/>
-    <hyperlink ref="C5" r:id="rId6" xr:uid="{BE061F6A-3915-469F-B564-0792F630E80B}"/>
-    <hyperlink ref="C6" r:id="rId7" xr:uid="{3383862E-8008-491B-B687-2194D47D7889}"/>
-    <hyperlink ref="C7" r:id="rId8" xr:uid="{FB307F13-8411-4B19-998F-8DE8B7D4F196}"/>
-    <hyperlink ref="C8" r:id="rId9" xr:uid="{1DCECA9C-7EC1-44CE-8D08-87B274779596}"/>
-    <hyperlink ref="C9" r:id="rId10" xr:uid="{21ADAF30-7FA3-46CA-A967-D8E497B97F43}"/>
-    <hyperlink ref="C10" r:id="rId11" xr:uid="{060BDDC4-A356-4192-9CF6-FBC8534EA411}"/>
-    <hyperlink ref="P3" r:id="rId12" xr:uid="{821CC43C-1313-4580-BDC6-70B8C7B0A4A7}"/>
-    <hyperlink ref="P4" r:id="rId13" xr:uid="{C2F111C0-95C6-4D8F-9C24-E46A71711A78}"/>
-    <hyperlink ref="P5" r:id="rId14" xr:uid="{38AF1568-3BEE-4963-8151-25BBD5DAD574}"/>
-    <hyperlink ref="P6" r:id="rId15" xr:uid="{3B4DBAE5-C9A9-4B9E-8413-857FEB4417F5}"/>
-    <hyperlink ref="P7" r:id="rId16" xr:uid="{CC977BE9-F0BD-4DE9-82C0-D35989737E4F}"/>
-    <hyperlink ref="P8" r:id="rId17" xr:uid="{9C9D1682-1878-4DA4-81B7-B6078F553A8E}"/>
-    <hyperlink ref="P9" r:id="rId18" xr:uid="{FE61339C-4D07-4138-8437-7D6DACCACF33}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{1A0B751A-EE31-44F8-BE4B-F6918B4B56D5}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{F706650C-E410-4E01-AB01-9A6E74B2CA2F}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{BE061F6A-3915-469F-B564-0792F630E80B}"/>
+    <hyperlink ref="C6" r:id="rId6" xr:uid="{3383862E-8008-491B-B687-2194D47D7889}"/>
+    <hyperlink ref="C7" r:id="rId7" xr:uid="{FB307F13-8411-4B19-998F-8DE8B7D4F196}"/>
+    <hyperlink ref="C8" r:id="rId8" xr:uid="{1DCECA9C-7EC1-44CE-8D08-87B274779596}"/>
+    <hyperlink ref="C9" r:id="rId9" xr:uid="{21ADAF30-7FA3-46CA-A967-D8E497B97F43}"/>
+    <hyperlink ref="C10" r:id="rId10" xr:uid="{060BDDC4-A356-4192-9CF6-FBC8534EA411}"/>
+    <hyperlink ref="P3" r:id="rId11" xr:uid="{821CC43C-1313-4580-BDC6-70B8C7B0A4A7}"/>
+    <hyperlink ref="P4" r:id="rId12" xr:uid="{C2F111C0-95C6-4D8F-9C24-E46A71711A78}"/>
+    <hyperlink ref="P5" r:id="rId13" xr:uid="{38AF1568-3BEE-4963-8151-25BBD5DAD574}"/>
+    <hyperlink ref="P6" r:id="rId14" xr:uid="{3B4DBAE5-C9A9-4B9E-8413-857FEB4417F5}"/>
+    <hyperlink ref="P7" r:id="rId15" xr:uid="{CC977BE9-F0BD-4DE9-82C0-D35989737E4F}"/>
+    <hyperlink ref="P8" r:id="rId16" xr:uid="{9C9D1682-1878-4DA4-81B7-B6078F553A8E}"/>
+    <hyperlink ref="P9" r:id="rId17" xr:uid="{FE61339C-4D07-4138-8437-7D6DACCACF33}"/>
+    <hyperlink ref="AJ2" r:id="rId18" xr:uid="{24BE68D4-CF69-482F-8590-D2EC761E3BC3}"/>
+    <hyperlink ref="AJ3" r:id="rId19" xr:uid="{576E65A5-0272-436C-91FD-0F782701E87C}"/>
+    <hyperlink ref="AJ4" r:id="rId20" xr:uid="{50D801F7-58E9-4DCD-A520-A64B1CF0A33D}"/>
+    <hyperlink ref="AJ5" r:id="rId21" xr:uid="{04AB1EB0-A863-49DD-918E-75891F10C075}"/>
+    <hyperlink ref="AJ6" r:id="rId22" xr:uid="{6D014992-1C26-47CC-BB15-EF707E6C3A99}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId19"/>
+  <legacyDrawing r:id="rId23"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B3A1E7-0A12-427B-8C9E-A9C2830C51A1}">
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="F1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5575,47 +5615,47 @@
       </c>
       <c r="H3" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>2.2999999999999998</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I3" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="J3" s="28">
         <f t="shared" ref="J3:R10" ca="1" si="0">ROUND(RAND()*5,1)</f>
-        <v>2.7</v>
+        <v>3.2</v>
       </c>
       <c r="K3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4000000000000004</v>
+        <v>3.4</v>
       </c>
       <c r="L3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="M3" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N3" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>2.1</v>
       </c>
-      <c r="N3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.7</v>
-      </c>
       <c r="O3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1</v>
+        <v>4.2</v>
       </c>
       <c r="P3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="Q3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3</v>
+        <v>3</v>
       </c>
       <c r="R3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5</v>
+        <v>0.3</v>
       </c>
       <c r="S3" t="s">
         <v>144</v>
@@ -5645,27 +5685,27 @@
       </c>
       <c r="H4" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>0.8</v>
+        <v>4.3</v>
       </c>
       <c r="I4" s="28">
         <f t="shared" ref="I4:I10" ca="1" si="1">ROUND(RAND()*5,1)</f>
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="J4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7</v>
+        <v>0.5</v>
       </c>
       <c r="K4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="L4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7</v>
+        <v>1.3</v>
       </c>
       <c r="M4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4000000000000004</v>
+        <v>0.9</v>
       </c>
       <c r="N4" s="28">
         <f t="shared" ca="1" si="0"/>
@@ -5673,19 +5713,19 @@
       </c>
       <c r="O4" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P4" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>1.8</v>
       </c>
-      <c r="P4" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.2</v>
-      </c>
       <c r="Q4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2.9</v>
       </c>
       <c r="R4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6</v>
+        <v>1.6</v>
       </c>
       <c r="S4" s="28" t="s">
         <v>153</v>
@@ -5719,43 +5759,43 @@
       </c>
       <c r="I5" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5999999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="J5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6</v>
+        <v>1.5</v>
       </c>
       <c r="K5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8</v>
+        <v>0.4</v>
       </c>
       <c r="L5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6</v>
+        <v>3.9</v>
       </c>
       <c r="M5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9</v>
+        <v>1.7</v>
       </c>
       <c r="N5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.3</v>
+        <v>0.7</v>
       </c>
       <c r="O5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4</v>
+        <v>2.6</v>
       </c>
       <c r="P5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1</v>
+        <v>2.7</v>
       </c>
       <c r="Q5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
       <c r="R5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3</v>
+        <v>3.5</v>
       </c>
       <c r="S5" s="28" t="s">
         <v>146</v>
@@ -5786,7 +5826,7 @@
       <c r="G6" s="17"/>
       <c r="H6" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>2.1</v>
+        <v>0.7</v>
       </c>
       <c r="I6" s="28">
         <f t="shared" ca="1" si="1"/>
@@ -5794,39 +5834,39 @@
       </c>
       <c r="J6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1</v>
+        <v>1</v>
       </c>
       <c r="K6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9</v>
+        <v>3.8</v>
       </c>
       <c r="L6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2.4</v>
       </c>
       <c r="M6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1</v>
+        <v>2.6</v>
       </c>
       <c r="N6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5</v>
+        <v>3.3</v>
       </c>
       <c r="O6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0999999999999996</v>
+        <v>0.2</v>
       </c>
       <c r="P6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9000000000000004</v>
+        <v>1.2</v>
       </c>
       <c r="Q6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="R6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8</v>
+        <v>3.5</v>
       </c>
       <c r="S6" s="28" t="s">
         <v>151</v>
@@ -5856,15 +5896,15 @@
       </c>
       <c r="H7" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>2.2000000000000002</v>
+        <v>3.3</v>
       </c>
       <c r="I7" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.3</v>
+        <v>2.8</v>
       </c>
       <c r="J7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6</v>
+        <v>3.8</v>
       </c>
       <c r="K7" s="28">
         <f t="shared" ca="1" si="0"/>
@@ -5872,27 +5912,27 @@
       </c>
       <c r="L7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5999999999999996</v>
+        <v>3</v>
       </c>
       <c r="M7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3.9</v>
       </c>
       <c r="N7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="O7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2</v>
+        <v>2.1</v>
       </c>
       <c r="P7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="Q7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2999999999999998</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="R7" s="28">
         <f t="shared" ca="1" si="0"/>
@@ -5926,47 +5966,47 @@
       </c>
       <c r="H8" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>2.4</v>
+        <v>0.8</v>
       </c>
       <c r="I8" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1000000000000001</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="J8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="K8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5999999999999996</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="L8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8</v>
+        <v>3.5</v>
       </c>
       <c r="M8" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="N8" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O8" s="28">
+        <f ca="1">ROUND(RAND()*5,1)</f>
         <v>3.3</v>
       </c>
-      <c r="N8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="O8" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.2</v>
-      </c>
       <c r="P8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1</v>
+        <v>1.5</v>
       </c>
       <c r="R8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1.7</v>
       </c>
       <c r="S8" s="28" t="s">
         <v>153</v>
@@ -5996,47 +6036,47 @@
       </c>
       <c r="H9" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>1.3</v>
+        <v>4.8</v>
       </c>
       <c r="I9" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4</v>
+        <v>1.2</v>
       </c>
       <c r="J9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8</v>
+        <v>0.1</v>
       </c>
       <c r="K9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8</v>
+        <v>3.8</v>
       </c>
       <c r="L9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1</v>
+        <v>2.9</v>
       </c>
       <c r="M9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="N9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7</v>
+        <v>0.7</v>
       </c>
       <c r="O9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="Q9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8</v>
+        <v>0.2</v>
       </c>
       <c r="R9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4</v>
+        <v>3.3</v>
       </c>
       <c r="S9" s="28" t="s">
         <v>145</v>
@@ -6052,6 +6092,9 @@
       <c r="B10" s="6">
         <v>1070653287</v>
       </c>
+      <c r="C10" t="s">
+        <v>169</v>
+      </c>
       <c r="D10">
         <v>3249900112</v>
       </c>
@@ -6063,47 +6106,47 @@
       </c>
       <c r="H10" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>4.8</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="I10" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>4.2</v>
+        <v>2.1</v>
       </c>
       <c r="J10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1</v>
+        <v>1.9</v>
       </c>
       <c r="K10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="L10" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>2.8</v>
+      </c>
+      <c r="M10" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.7</v>
+      </c>
+      <c r="N10" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="O10" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="P10" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.1</v>
+      </c>
+      <c r="Q10" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.3</v>
+      </c>
+      <c r="R10" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>4.7</v>
-      </c>
-      <c r="M10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.9</v>
-      </c>
-      <c r="N10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.8</v>
-      </c>
-      <c r="O10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.5</v>
-      </c>
-      <c r="P10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.7</v>
-      </c>
-      <c r="Q10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="R10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.4</v>
       </c>
       <c r="S10" s="28" t="s">
         <v>153</v>
@@ -6241,59 +6284,67 @@
       <c r="B13">
         <v>1023456789</v>
       </c>
+      <c r="C13" t="s">
+        <v>71</v>
+      </c>
       <c r="D13">
         <v>3101234567</v>
       </c>
       <c r="E13">
         <v>3155551212</v>
       </c>
-      <c r="F13" s="30"/>
+      <c r="F13" s="27" t="s">
+        <v>170</v>
+      </c>
       <c r="H13">
-        <f t="shared" ref="H13:R16" ca="1" si="3">ROUND(RAND()*5,1)</f>
-        <v>4.5</v>
+        <f t="shared" ref="H13:R18" ca="1" si="3">ROUND(RAND()*5,1)</f>
+        <v>1.7</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="3"/>
-        <v>0.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="3"/>
-        <v>3.6</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="3"/>
-        <v>1.3</v>
+        <v>0.1</v>
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="3"/>
-        <v>3.6</v>
+        <v>1.2</v>
       </c>
       <c r="M13">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>0.9</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="3"/>
-        <v>3.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="O13">
         <f t="shared" ca="1" si="3"/>
-        <v>4.4000000000000004</v>
+        <v>2.8</v>
       </c>
       <c r="P13">
         <f t="shared" ca="1" si="3"/>
-        <v>1.1000000000000001</v>
+        <v>1.9</v>
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="3"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="R13">
         <f t="shared" ca="1" si="3"/>
-        <v>1.5</v>
+        <v>0.2</v>
       </c>
       <c r="S13" s="37" t="s">
         <v>144</v>
+      </c>
+      <c r="T13" s="29" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -6303,20 +6354,25 @@
       <c r="B14">
         <v>1122334455</v>
       </c>
+      <c r="C14" s="28" t="s">
+        <v>160</v>
+      </c>
       <c r="D14">
         <v>3112223344</v>
       </c>
       <c r="E14">
         <v>3224445566</v>
       </c>
-      <c r="F14" s="30"/>
+      <c r="F14" s="27" t="s">
+        <v>171</v>
+      </c>
       <c r="H14">
         <f t="shared" ca="1" si="3"/>
-        <v>2.1</v>
+        <v>4.2</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="3"/>
-        <v>0.8</v>
+        <v>4.3</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="3"/>
@@ -6324,38 +6380,41 @@
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9</v>
+        <v>3.2</v>
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="3"/>
-        <v>1.5</v>
+        <v>0.2</v>
       </c>
       <c r="M14">
         <f t="shared" ca="1" si="3"/>
-        <v>2.5</v>
+        <v>1.7</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="3"/>
-        <v>1.6</v>
+        <v>1.2</v>
       </c>
       <c r="O14">
         <f t="shared" ca="1" si="3"/>
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="P14">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="3"/>
-        <v>3.7</v>
+        <v>3.6</v>
       </c>
       <c r="R14">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="S14" t="s">
         <v>147</v>
+      </c>
+      <c r="T14" s="29" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -6365,58 +6424,67 @@
       <c r="B15">
         <v>1234567890</v>
       </c>
+      <c r="C15" s="28" t="s">
+        <v>162</v>
+      </c>
       <c r="D15">
         <v>3007778899</v>
       </c>
       <c r="E15">
         <v>3129991122</v>
       </c>
+      <c r="F15" s="27" t="s">
+        <v>172</v>
+      </c>
       <c r="H15">
         <f t="shared" ca="1" si="3"/>
-        <v>4.8</v>
+        <v>3.1</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="3"/>
-        <v>4.8</v>
+        <v>1.3</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="3"/>
-        <v>4.8</v>
+        <v>3.9</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9</v>
+        <v>1</v>
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="3"/>
-        <v>4.4000000000000004</v>
+        <v>3.1</v>
       </c>
       <c r="M15">
         <f t="shared" ca="1" si="3"/>
-        <v>3.6</v>
+        <v>0.3</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="3"/>
-        <v>1.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="O15">
         <f t="shared" ca="1" si="3"/>
-        <v>2.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="P15">
         <f t="shared" ca="1" si="3"/>
-        <v>3.2</v>
+        <v>3.8</v>
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="3"/>
-        <v>0.2</v>
+        <v>3.5</v>
       </c>
       <c r="R15">
         <f t="shared" ca="1" si="3"/>
-        <v>3.6</v>
+        <v>1.5</v>
       </c>
       <c r="S15" t="s">
         <v>145</v>
+      </c>
+      <c r="T15" s="29" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -6426,63 +6494,209 @@
       <c r="B16" s="18">
         <v>1098765432</v>
       </c>
-      <c r="C16" s="17"/>
+      <c r="C16" s="28" t="s">
+        <v>161</v>
+      </c>
       <c r="D16" s="17">
         <v>3173344556</v>
       </c>
       <c r="E16" s="17">
         <v>3195566778</v>
       </c>
-      <c r="F16" s="17"/>
+      <c r="F16" s="27" t="s">
+        <v>173</v>
+      </c>
       <c r="G16" s="17"/>
       <c r="H16" s="18">
         <f t="shared" ca="1" si="3"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I16">
+        <f t="shared" ca="1" si="3"/>
+        <v>2.6</v>
+      </c>
+      <c r="J16">
+        <f t="shared" ca="1" si="3"/>
+        <v>4.8</v>
+      </c>
+      <c r="K16">
+        <f t="shared" ca="1" si="3"/>
+        <v>1.8</v>
+      </c>
+      <c r="L16">
+        <f t="shared" ca="1" si="3"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M16">
+        <f t="shared" ca="1" si="3"/>
+        <v>1.5</v>
+      </c>
+      <c r="N16">
+        <f t="shared" ca="1" si="3"/>
+        <v>2.5</v>
+      </c>
+      <c r="O16">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="P16">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.4</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" ca="1" si="3"/>
+        <v>2.5</v>
+      </c>
+      <c r="R16">
+        <f t="shared" ca="1" si="3"/>
         <v>3.2</v>
       </c>
-      <c r="I16" s="18">
+      <c r="S16" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="T16" s="29" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17">
+        <v>1000939523</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="D17">
+        <v>3216677889</v>
+      </c>
+      <c r="E17">
+        <v>3184455667</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="H17" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>0.1</v>
-      </c>
-      <c r="J16" s="18">
-        <f t="shared" ca="1" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="K16" s="18">
+        <v>4</v>
+      </c>
+      <c r="I17">
         <f t="shared" ca="1" si="3"/>
         <v>3.8</v>
       </c>
-      <c r="L16" s="18">
+      <c r="J17">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9</v>
-      </c>
-      <c r="M16" s="18">
+        <v>4.3</v>
+      </c>
+      <c r="K17">
+        <f t="shared" ca="1" si="3"/>
+        <v>4.3</v>
+      </c>
+      <c r="L17">
+        <f t="shared" ca="1" si="3"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="M17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.7</v>
+      </c>
+      <c r="N17">
         <f t="shared" ca="1" si="3"/>
         <v>3.1</v>
       </c>
-      <c r="N16" s="18">
-        <f t="shared" ca="1" si="3"/>
-        <v>2.4</v>
-      </c>
-      <c r="O16" s="18">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="P16" s="18">
-        <f t="shared" ca="1" si="3"/>
-        <v>4.5</v>
-      </c>
-      <c r="Q16" s="18">
+      <c r="O17">
         <f t="shared" ca="1" si="3"/>
         <v>3.8</v>
       </c>
-      <c r="R16" s="18">
+      <c r="P17">
         <f t="shared" ca="1" si="3"/>
-        <v>1.4</v>
-      </c>
-      <c r="S16" s="18" t="s">
+        <v>1.8</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" ca="1" si="3"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="R17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="S17" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="T16" s="18"/>
+      <c r="T17" s="29" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>134</v>
+      </c>
+      <c r="B18">
+        <v>1928412412</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18">
+        <v>3237788990</v>
+      </c>
+      <c r="E18">
+        <v>3248899001</v>
+      </c>
+      <c r="F18" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="H18" s="18">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.7</v>
+      </c>
+      <c r="I18" s="18">
+        <f ca="1">ROUND(RAND()*5,1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="J18" s="18">
+        <f ca="1">ROUND(RAND()*5,1)</f>
+        <v>4.5</v>
+      </c>
+      <c r="K18" s="18">
+        <f ca="1">ROUND(RAND()*5,1)</f>
+        <v>2.8</v>
+      </c>
+      <c r="L18" s="18">
+        <f ca="1">ROUND(RAND()*5,1)</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M18" s="18">
+        <f ca="1">ROUND(RAND()*5,1)</f>
+        <v>0.1</v>
+      </c>
+      <c r="N18" s="18">
+        <f ca="1">ROUND(RAND()*5,1)</f>
+        <v>1.9</v>
+      </c>
+      <c r="O18" s="18">
+        <f ca="1">ROUND(RAND()*5,1)</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="P18" s="18">
+        <f ca="1">ROUND(RAND()*5,1)</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="Q18" s="18">
+        <f ca="1">ROUND(RAND()*5,1)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R18" s="18">
+        <f ca="1">ROUND(RAND()*5,1)</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="S18" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="T18" s="29" t="s">
+        <v>150</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:B1">
@@ -6534,9 +6748,16 @@
     <hyperlink ref="F8" r:id="rId7" xr:uid="{9EF2539C-5D0C-4259-AEFE-801473A4AF2B}"/>
     <hyperlink ref="F9" r:id="rId8" xr:uid="{28EF3113-8C25-4D27-82F7-A2C9B1CB8D47}"/>
     <hyperlink ref="F12" r:id="rId9" xr:uid="{86CE8B1E-8882-41D3-98CF-894BC1DCA683}"/>
+    <hyperlink ref="F13" r:id="rId10" xr:uid="{3D890F57-5D7C-4E65-85D4-00CADB43EE64}"/>
+    <hyperlink ref="F14" r:id="rId11" xr:uid="{0B72E832-BAC4-4EE8-934C-306B979BFB8D}"/>
+    <hyperlink ref="F15" r:id="rId12" xr:uid="{23EB530F-65DC-47A9-A53C-F6A7C9B78C34}"/>
+    <hyperlink ref="F16" r:id="rId13" xr:uid="{10443379-01B0-4414-8F08-13C234E0FE03}"/>
+    <hyperlink ref="F17:F18" r:id="rId14" display="CorreoEjemplo555@gmail.com" xr:uid="{BBA3B62B-41AA-4B4D-B220-5FEE22909FF5}"/>
+    <hyperlink ref="F17" r:id="rId15" xr:uid="{9F52F163-52EC-4037-9214-AFB274DA45DA}"/>
+    <hyperlink ref="F18" r:id="rId16" xr:uid="{10C3BEAF-34A4-4A62-8C36-9188D2826DA7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId10"/>
+  <legacyDrawing r:id="rId17"/>
 </worksheet>
 </file>
 
@@ -6771,19 +6992,19 @@
     <cfRule type="duplicateValues" dxfId="33" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:G1">
-    <cfRule type="duplicateValues" dxfId="32" priority="53"/>
-    <cfRule type="duplicateValues" dxfId="31" priority="52"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="52"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:K1">
-    <cfRule type="duplicateValues" dxfId="30" priority="30"/>
-    <cfRule type="duplicateValues" dxfId="29" priority="21"/>
-    <cfRule type="duplicateValues" dxfId="28" priority="31"/>
-    <cfRule type="duplicateValues" dxfId="27" priority="23"/>
-    <cfRule type="duplicateValues" dxfId="26" priority="24"/>
-    <cfRule type="duplicateValues" dxfId="25" priority="25"/>
-    <cfRule type="duplicateValues" dxfId="24" priority="26"/>
-    <cfRule type="duplicateValues" dxfId="23" priority="35"/>
-    <cfRule type="duplicateValues" dxfId="22" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1">
     <cfRule type="duplicateValues" dxfId="21" priority="37"/>
@@ -6792,13 +7013,13 @@
     <cfRule type="duplicateValues" dxfId="20" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB1:AC1">
-    <cfRule type="duplicateValues" dxfId="19" priority="27"/>
-    <cfRule type="duplicateValues" dxfId="18" priority="28"/>
-    <cfRule type="duplicateValues" dxfId="17" priority="29"/>
-    <cfRule type="duplicateValues" dxfId="16" priority="33"/>
-    <cfRule type="duplicateValues" dxfId="15" priority="36"/>
-    <cfRule type="duplicateValues" dxfId="14" priority="20"/>
-    <cfRule type="duplicateValues" dxfId="13" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC1">
     <cfRule type="duplicateValues" dxfId="12" priority="19"/>

</xml_diff>

<commit_message>
:white_check_mark: Prueba de aceptación #2.
</commit_message>
<xml_diff>
--- a/recursos/EmparejamientoFINAL.xlsx
+++ b/recursos/EmparejamientoFINAL.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\OneDrive\Documents\7 semestre\Sistema-TuGestor\recursos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\Sistema-TuGestor\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B36BCE5-7918-4734-9315-C24F8CF79723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C333FCF7-D9F5-4417-979A-464BD90ED6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="670" xr2:uid="{FD9F6918-DD5F-4EFB-A5DA-81B3D2DC95CD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="670" xr2:uid="{FD9F6918-DD5F-4EFB-A5DA-81B3D2DC95CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Emparejamiento" sheetId="1" r:id="rId1"/>
@@ -29,17 +29,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -52,10 +41,19 @@
   <commentList>
     <comment ref="AE2" authorId="0" shapeId="0" xr:uid="{1CDBB0FC-D22E-4D10-A2DB-DC4D443F4280}">
       <text>
-        <t>[Comentario encadenado]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     Tuvo problemas de salud y no se ha contactado a las tutorías, pendiente respuesta para avisar al tutor</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -70,10 +68,19 @@
   <commentList>
     <comment ref="A12" authorId="0" shapeId="0" xr:uid="{B30B35B7-16C6-42C1-8BFB-C43D8A401A3B}">
       <text>
-        <t>[Comentario encadenado]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     Tuvo problemas de salud y no se ha contactado a las tutorías, pendiente respuesta para avisar al tutor</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -987,6 +994,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1047,26 +1074,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1077,16 +1084,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1097,6 +1094,56 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1107,6 +1154,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1127,6 +1184,146 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1167,151 +1364,121 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1337,6 +1504,146 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1377,86 +1684,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1467,6 +1694,76 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1477,6 +1774,126 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1497,6 +1914,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1507,156 +1934,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1672,276 +1949,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2420,7 +2427,7 @@
   <dimension ref="A1:AZ57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2808,48 +2815,47 @@
         <v>143</v>
       </c>
       <c r="R3" s="28">
-        <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>3.9</v>
+        <v>1</v>
       </c>
       <c r="S3" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>4.9000000000000004</v>
+        <v>0.8</v>
       </c>
       <c r="T3" s="28">
         <f t="shared" ref="T3:AB10" ca="1" si="0">ROUND(RAND()*5,1)</f>
-        <v>0.9</v>
+        <v>3</v>
       </c>
       <c r="U3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1.6</v>
       </c>
       <c r="V3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2000000000000002</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="W3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2999999999999998</v>
+        <v>0.3</v>
       </c>
       <c r="X3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7</v>
+        <v>1.3</v>
       </c>
       <c r="Y3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="Z3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2999999999999998</v>
+        <v>4.7</v>
       </c>
       <c r="AA3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8</v>
+        <v>1.9</v>
       </c>
       <c r="AB3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5</v>
+        <v>3.9</v>
       </c>
       <c r="AC3" t="s">
         <v>144</v>
@@ -2880,11 +2886,11 @@
       </c>
       <c r="AL3">
         <f t="shared" ref="AL3:AV8" ca="1" si="1">ROUND(RAND()*5,1)</f>
-        <v>4.2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="AM3">
         <f t="shared" ca="1" si="1"/>
-        <v>4.8</v>
+        <v>2.1</v>
       </c>
       <c r="AN3">
         <f t="shared" ca="1" si="1"/>
@@ -2892,35 +2898,35 @@
       </c>
       <c r="AO3">
         <f t="shared" ca="1" si="1"/>
-        <v>0.1</v>
+        <v>2.6</v>
       </c>
       <c r="AP3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1000000000000001</v>
+        <v>1.7</v>
       </c>
       <c r="AQ3">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2</v>
+        <v>3.2</v>
       </c>
       <c r="AR3">
         <f t="shared" ca="1" si="1"/>
-        <v>0.5</v>
+        <v>3.1</v>
       </c>
       <c r="AS3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.3</v>
+        <v>3.9</v>
       </c>
       <c r="AT3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="AU3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.3</v>
+        <v>0.2</v>
       </c>
       <c r="AV3">
         <f t="shared" ca="1" si="1"/>
-        <v>3.4</v>
+        <v>2.7</v>
       </c>
       <c r="AW3" s="37" t="s">
         <v>144</v>
@@ -2989,47 +2995,47 @@
       </c>
       <c r="R4" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>4.8</v>
+        <v>1.3</v>
       </c>
       <c r="S4" s="28">
         <f t="shared" ref="S4:S10" ca="1" si="2">ROUND(RAND()*5,1)</f>
-        <v>3.6</v>
+        <v>3</v>
       </c>
       <c r="T4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2000000000000002</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="U4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7</v>
+        <v>4</v>
       </c>
       <c r="V4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9000000000000004</v>
+        <v>1.9</v>
       </c>
       <c r="W4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1</v>
+        <v>3.3</v>
       </c>
       <c r="X4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9000000000000004</v>
+        <v>3.4</v>
       </c>
       <c r="Y4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
       <c r="Z4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1</v>
+        <v>4.5</v>
       </c>
       <c r="AA4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5</v>
+        <v>3.1</v>
       </c>
       <c r="AB4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6</v>
+        <v>3.2</v>
       </c>
       <c r="AC4" s="28" t="s">
         <v>153</v>
@@ -3060,47 +3066,47 @@
       </c>
       <c r="AL4">
         <f t="shared" ca="1" si="1"/>
-        <v>4.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AM4">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AN4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.8</v>
+        <v>4.5</v>
       </c>
       <c r="AO4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2999999999999998</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="AP4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1</v>
+        <v>4.3</v>
       </c>
       <c r="AQ4">
         <f t="shared" ca="1" si="1"/>
-        <v>3.7</v>
+        <v>1.6</v>
       </c>
       <c r="AR4">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="AS4">
         <f t="shared" ca="1" si="1"/>
-        <v>3.5</v>
+        <v>2.1</v>
       </c>
       <c r="AT4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4</v>
+        <v>2.7</v>
       </c>
       <c r="AU4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2.8</v>
       </c>
       <c r="AV4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2999999999999998</v>
+        <v>3.9</v>
       </c>
       <c r="AW4" t="s">
         <v>147</v>
@@ -3169,47 +3175,47 @@
       </c>
       <c r="R5" s="28">
         <f t="shared" ref="R5:R10" ca="1" si="3">ROUND(RAND()*5,1)</f>
-        <v>4.0999999999999996</v>
+        <v>2.8</v>
       </c>
       <c r="S5" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>2.6</v>
+        <v>1</v>
       </c>
       <c r="T5" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>3.8</v>
+      </c>
+      <c r="U5" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="V5" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>4.5</v>
       </c>
-      <c r="U5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.7</v>
-      </c>
-      <c r="V5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
       <c r="W5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="X5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8</v>
+        <v>3.2</v>
       </c>
       <c r="Y5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6</v>
+        <v>2.7</v>
       </c>
       <c r="Z5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2</v>
+        <v>4.2</v>
       </c>
       <c r="AA5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2</v>
+        <v>0.3</v>
       </c>
       <c r="AB5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8</v>
+        <v>4.3</v>
       </c>
       <c r="AC5" s="28" t="s">
         <v>146</v>
@@ -3240,27 +3246,27 @@
       </c>
       <c r="AL5">
         <f t="shared" ca="1" si="1"/>
-        <v>4.8</v>
+        <v>2.7</v>
       </c>
       <c r="AM5">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6</v>
+        <v>4.2</v>
       </c>
       <c r="AN5">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="AO5">
         <f t="shared" ca="1" si="1"/>
-        <v>2.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="AP5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.1</v>
+        <v>3.9</v>
       </c>
       <c r="AQ5">
         <f t="shared" ca="1" si="1"/>
-        <v>2.6</v>
+        <v>3.2</v>
       </c>
       <c r="AR5">
         <f t="shared" ca="1" si="1"/>
@@ -3268,19 +3274,19 @@
       </c>
       <c r="AS5">
         <f t="shared" ca="1" si="1"/>
-        <v>1.5</v>
+        <v>0.1</v>
       </c>
       <c r="AT5">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5</v>
+        <v>1.8</v>
       </c>
       <c r="AU5">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="AV5">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5</v>
+        <v>1.8</v>
       </c>
       <c r="AW5" t="s">
         <v>145</v>
@@ -3349,47 +3355,47 @@
       </c>
       <c r="R6" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="S6" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>1.6</v>
+        <v>3.1</v>
       </c>
       <c r="T6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5</v>
+        <v>3.7</v>
       </c>
       <c r="U6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="V6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
       <c r="W6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8</v>
+        <v>0.4</v>
       </c>
       <c r="X6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2</v>
+        <v>3.2</v>
       </c>
       <c r="Y6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="Z6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0999999999999996</v>
+        <v>2.4</v>
       </c>
       <c r="AA6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0999999999999996</v>
+        <v>3.1</v>
       </c>
       <c r="AB6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1</v>
+        <v>2.5</v>
       </c>
       <c r="AC6" s="28" t="s">
         <v>151</v>
@@ -3420,47 +3426,47 @@
       </c>
       <c r="AL6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.1</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="AM6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>4.3</v>
+        <v>0.9</v>
       </c>
       <c r="AN6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2999999999999998</v>
+        <v>2.1</v>
       </c>
       <c r="AO6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8</v>
+        <v>3.4</v>
       </c>
       <c r="AP6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7</v>
+        <v>1.2</v>
       </c>
       <c r="AQ6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.9</v>
+        <v>4.7</v>
       </c>
       <c r="AR6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.7</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="AS6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>3.4</v>
+        <v>0.7</v>
       </c>
       <c r="AT6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>4.7</v>
       </c>
       <c r="AU6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2</v>
+        <v>1.4</v>
       </c>
       <c r="AV6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>3.1</v>
+        <v>3.7</v>
       </c>
       <c r="AW6" s="18" t="s">
         <v>152</v>
@@ -3529,47 +3535,47 @@
       </c>
       <c r="R7" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="S7" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="T7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8</v>
+        <v>1</v>
       </c>
       <c r="U7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7</v>
+        <v>3.7</v>
       </c>
       <c r="V7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1000000000000001</v>
+        <v>0.3</v>
       </c>
       <c r="W7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7</v>
+        <v>0.2</v>
       </c>
       <c r="X7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5</v>
+        <v>3.7</v>
       </c>
       <c r="Y7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4</v>
+        <v>4.2</v>
       </c>
       <c r="Z7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="AA7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7</v>
+        <v>3.6</v>
       </c>
       <c r="AB7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4</v>
+        <v>3.7</v>
       </c>
       <c r="AC7" s="28" t="s">
         <v>145</v>
@@ -3597,47 +3603,47 @@
       </c>
       <c r="AL7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="AM7">
         <f t="shared" ca="1" si="1"/>
-        <v>3.2</v>
+        <v>2.6</v>
       </c>
       <c r="AN7">
         <f t="shared" ca="1" si="1"/>
-        <v>3.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="AO7">
         <f t="shared" ca="1" si="1"/>
-        <v>4.2</v>
+        <v>3</v>
       </c>
       <c r="AP7">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7</v>
+        <v>4.2</v>
       </c>
       <c r="AQ7">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2</v>
+        <v>0.2</v>
       </c>
       <c r="AR7">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="AS7">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5999999999999996</v>
+        <v>0.2</v>
       </c>
       <c r="AT7">
         <f t="shared" ca="1" si="1"/>
-        <v>4.8</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="AU7">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5</v>
+        <v>1.3</v>
       </c>
       <c r="AV7">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1.6</v>
       </c>
       <c r="AW7" t="s">
         <v>144</v>
@@ -3706,39 +3712,39 @@
       </c>
       <c r="R8" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>2.8</v>
+        <v>1.6</v>
       </c>
       <c r="S8" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>3.4</v>
+        <v>0.7</v>
       </c>
       <c r="T8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4</v>
+        <v>2.5</v>
       </c>
       <c r="U8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7</v>
+        <v>2.8</v>
       </c>
       <c r="V8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4</v>
+        <v>0.1</v>
       </c>
       <c r="W8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5999999999999996</v>
+        <v>0.6</v>
       </c>
       <c r="X8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9</v>
+        <v>4</v>
       </c>
       <c r="Y8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9</v>
+        <v>0.3</v>
       </c>
       <c r="Z8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4</v>
+        <v>4.8</v>
       </c>
       <c r="AA8" s="28">
         <f t="shared" ca="1" si="0"/>
@@ -3746,7 +3752,7 @@
       </c>
       <c r="AB8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4</v>
+        <v>0.2</v>
       </c>
       <c r="AC8" s="28" t="s">
         <v>153</v>
@@ -3774,47 +3780,47 @@
       </c>
       <c r="AL8">
         <f t="shared" ca="1" si="1"/>
-        <v>3.7</v>
+        <v>2</v>
       </c>
       <c r="AM8">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1.7</v>
       </c>
       <c r="AN8">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2000000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="AO8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.7</v>
+        <v>3.3</v>
       </c>
       <c r="AP8">
         <f t="shared" ca="1" si="1"/>
-        <v>3.6</v>
+        <v>4.5</v>
       </c>
       <c r="AQ8">
         <f t="shared" ca="1" si="1"/>
-        <v>3.8</v>
+        <v>1.9</v>
       </c>
       <c r="AR8">
         <f t="shared" ca="1" si="1"/>
-        <v>4.8</v>
+        <v>2.1</v>
       </c>
       <c r="AS8">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="AT8">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7</v>
+        <v>0.5</v>
       </c>
       <c r="AU8">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>0.1</v>
       </c>
       <c r="AV8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.3</v>
+        <v>2.7</v>
       </c>
       <c r="AW8" t="s">
         <v>152</v>
@@ -3883,47 +3889,47 @@
       </c>
       <c r="R9" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>3.9</v>
+        <v>3.7</v>
       </c>
       <c r="S9" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>2.2000000000000002</v>
+        <v>4.2</v>
       </c>
       <c r="T9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8</v>
+        <v>4.5</v>
       </c>
       <c r="U9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4</v>
+        <v>2.5</v>
       </c>
       <c r="V9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="W9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5</v>
+        <v>3.2</v>
       </c>
       <c r="X9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Y9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5</v>
+        <v>3.9</v>
       </c>
       <c r="Z9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4000000000000004</v>
+        <v>1.7</v>
       </c>
       <c r="AA9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3</v>
+        <v>1.7</v>
       </c>
       <c r="AB9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2</v>
+        <v>2.8</v>
       </c>
       <c r="AC9" s="28" t="s">
         <v>145</v>
@@ -3987,19 +3993,19 @@
       </c>
       <c r="R10" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>1.2</v>
+        <v>0.2</v>
       </c>
       <c r="S10" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>1.1000000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="T10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>0.9</v>
       </c>
       <c r="U10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9</v>
+        <v>3.2</v>
       </c>
       <c r="V10" s="28">
         <f t="shared" ca="1" si="0"/>
@@ -4007,11 +4013,11 @@
       </c>
       <c r="W10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5</v>
+        <v>4.2</v>
       </c>
       <c r="X10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>0.7</v>
       </c>
       <c r="Y10" s="28">
         <f t="shared" ca="1" si="0"/>
@@ -4023,11 +4029,11 @@
       </c>
       <c r="AA10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7</v>
+        <v>0.4</v>
       </c>
       <c r="AB10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.3</v>
+        <v>4.5</v>
       </c>
       <c r="AC10" s="28" t="s">
         <v>153</v>
@@ -5325,25 +5331,25 @@
     <cfRule type="duplicateValues" dxfId="120" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:G1">
-    <cfRule type="duplicateValues" dxfId="119" priority="72"/>
-    <cfRule type="duplicateValues" dxfId="118" priority="73"/>
-    <cfRule type="duplicateValues" dxfId="117" priority="74"/>
-    <cfRule type="duplicateValues" dxfId="116" priority="75"/>
-    <cfRule type="duplicateValues" dxfId="115" priority="76"/>
-    <cfRule type="duplicateValues" dxfId="114" priority="77"/>
-    <cfRule type="duplicateValues" dxfId="113" priority="84"/>
-    <cfRule type="duplicateValues" dxfId="112" priority="85"/>
+    <cfRule type="duplicateValues" dxfId="119" priority="84"/>
+    <cfRule type="duplicateValues" dxfId="118" priority="77"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="85"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="76"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="75"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="74"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="72"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="73"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:L1">
-    <cfRule type="duplicateValues" dxfId="111" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="42"/>
     <cfRule type="duplicateValues" dxfId="110" priority="41"/>
-    <cfRule type="duplicateValues" dxfId="109" priority="42"/>
-    <cfRule type="duplicateValues" dxfId="108" priority="43"/>
-    <cfRule type="duplicateValues" dxfId="107" priority="44"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="52"/>
+    <cfRule type="duplicateValues" dxfId="107" priority="49"/>
     <cfRule type="duplicateValues" dxfId="106" priority="48"/>
-    <cfRule type="duplicateValues" dxfId="105" priority="49"/>
-    <cfRule type="duplicateValues" dxfId="104" priority="52"/>
-    <cfRule type="duplicateValues" dxfId="103" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="105" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="104" priority="44"/>
+    <cfRule type="duplicateValues" dxfId="103" priority="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:L6">
     <cfRule type="duplicateValues" dxfId="102" priority="15"/>
@@ -5394,13 +5400,13 @@
     <cfRule type="duplicateValues" dxfId="87" priority="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE1:AF1">
-    <cfRule type="duplicateValues" dxfId="86" priority="38"/>
-    <cfRule type="duplicateValues" dxfId="85" priority="40"/>
-    <cfRule type="duplicateValues" dxfId="84" priority="45"/>
-    <cfRule type="duplicateValues" dxfId="83" priority="46"/>
-    <cfRule type="duplicateValues" dxfId="82" priority="47"/>
-    <cfRule type="duplicateValues" dxfId="81" priority="51"/>
-    <cfRule type="duplicateValues" dxfId="80" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="86" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="85" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="84" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="83" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="82" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="81" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="80" priority="51"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE2:AF2 K7:L18 L5:M6 K3:L5">
     <cfRule type="duplicateValues" dxfId="79" priority="36"/>
@@ -5615,47 +5621,47 @@
       </c>
       <c r="H3" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>4.9000000000000004</v>
+        <v>3.2</v>
       </c>
       <c r="I3" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>0.5</v>
+        <v>3.4</v>
       </c>
       <c r="J3" s="28">
         <f t="shared" ref="J3:R10" ca="1" si="0">ROUND(RAND()*5,1)</f>
-        <v>3.2</v>
+        <v>4</v>
       </c>
       <c r="K3" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>3.8</v>
+      </c>
+      <c r="L3" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.4</v>
+      </c>
+      <c r="M3" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="N3" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="O3" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="P3" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.7</v>
+      </c>
+      <c r="Q3" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R3" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>3.4</v>
-      </c>
-      <c r="L3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.9</v>
-      </c>
-      <c r="M3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="N3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.1</v>
-      </c>
-      <c r="O3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.2</v>
-      </c>
-      <c r="P3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="Q3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="R3" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.3</v>
       </c>
       <c r="S3" t="s">
         <v>144</v>
@@ -5685,47 +5691,47 @@
       </c>
       <c r="H4" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>4.3</v>
+        <v>2</v>
       </c>
       <c r="I4" s="28">
         <f t="shared" ref="I4:I10" ca="1" si="1">ROUND(RAND()*5,1)</f>
-        <v>2.5</v>
+        <v>1.3</v>
       </c>
       <c r="J4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5</v>
+        <v>3.1</v>
       </c>
       <c r="K4" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>2.8</v>
+      </c>
+      <c r="L4" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M4" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>3.4</v>
       </c>
-      <c r="L4" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.3</v>
-      </c>
-      <c r="M4" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.9</v>
-      </c>
       <c r="N4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6</v>
+        <v>4.5</v>
       </c>
       <c r="O4" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="P4" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="Q4" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="P4" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.8</v>
-      </c>
-      <c r="Q4" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.9</v>
-      </c>
       <c r="R4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6</v>
+        <v>4.3</v>
       </c>
       <c r="S4" s="28" t="s">
         <v>153</v>
@@ -5755,47 +5761,47 @@
       </c>
       <c r="H5" s="28">
         <f t="shared" ref="H5:H10" ca="1" si="2">ROUND(RAND()*5,1)</f>
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I5" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="J5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="K5" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>3.9</v>
+      </c>
+      <c r="L5" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="L5" s="28">
+      <c r="M5" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="N5" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.6</v>
+      </c>
+      <c r="O5" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="P5" s="28">
         <f t="shared" ca="1" si="0"/>
         <v>3.9</v>
       </c>
-      <c r="M5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.7</v>
-      </c>
-      <c r="N5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.7</v>
-      </c>
-      <c r="O5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.6</v>
-      </c>
-      <c r="P5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.7</v>
-      </c>
       <c r="Q5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
       <c r="R5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="S5" s="28" t="s">
         <v>146</v>
@@ -5826,47 +5832,47 @@
       <c r="G6" s="17"/>
       <c r="H6" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>0.7</v>
+        <v>2.4</v>
       </c>
       <c r="I6" s="28">
         <f t="shared" ca="1" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="J6" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="K6" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="L6" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M6" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>3.6</v>
       </c>
-      <c r="J6" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K6" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.8</v>
-      </c>
-      <c r="L6" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.4</v>
-      </c>
-      <c r="M6" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.6</v>
-      </c>
       <c r="N6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3</v>
+        <v>1.6</v>
       </c>
       <c r="O6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2</v>
+        <v>2.9</v>
       </c>
       <c r="P6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="Q6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="R6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5</v>
+        <v>2.7</v>
       </c>
       <c r="S6" s="28" t="s">
         <v>151</v>
@@ -5896,47 +5902,47 @@
       </c>
       <c r="H7" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>3.3</v>
+        <v>1.3</v>
       </c>
       <c r="I7" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>2.8</v>
+        <v>0.4</v>
       </c>
       <c r="J7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8</v>
+        <v>0.4</v>
       </c>
       <c r="K7" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="L7" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.1</v>
+      </c>
+      <c r="M7" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.1</v>
+      </c>
+      <c r="N7" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>4.7</v>
       </c>
-      <c r="L7" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="M7" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.9</v>
-      </c>
-      <c r="N7" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.2000000000000002</v>
-      </c>
       <c r="O7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1</v>
+        <v>1</v>
       </c>
       <c r="P7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0999999999999996</v>
+        <v>2.7</v>
       </c>
       <c r="Q7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0999999999999996</v>
+        <v>3.4</v>
       </c>
       <c r="R7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="S7" s="28" t="s">
         <v>145</v>
@@ -5966,47 +5972,47 @@
       </c>
       <c r="H8" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8</v>
+        <v>3.6</v>
       </c>
       <c r="I8" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2000000000000002</v>
+        <v>3.6</v>
       </c>
       <c r="J8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="K8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2000000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="L8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5</v>
+        <v>0.8</v>
       </c>
       <c r="M8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9000000000000004</v>
+        <v>0.2</v>
       </c>
       <c r="N8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="O8" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>3.3</v>
+        <v>4.8</v>
       </c>
       <c r="P8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="Q8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5</v>
+        <v>3.4</v>
       </c>
       <c r="R8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7</v>
+        <v>2.8</v>
       </c>
       <c r="S8" s="28" t="s">
         <v>153</v>
@@ -6036,47 +6042,47 @@
       </c>
       <c r="H9" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>4.8</v>
+        <v>3.2</v>
       </c>
       <c r="I9" s="28">
         <f t="shared" ca="1" si="1"/>
+        <v>3.5</v>
+      </c>
+      <c r="J9" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="K9" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="L9" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.6</v>
+      </c>
+      <c r="M9" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>1.2</v>
       </c>
-      <c r="J9" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="K9" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.8</v>
-      </c>
-      <c r="L9" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.9</v>
-      </c>
-      <c r="M9" s="28">
+      <c r="N9" s="28">
         <f t="shared" ca="1" si="0"/>
         <v>4.4000000000000004</v>
       </c>
-      <c r="N9" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.7</v>
-      </c>
       <c r="O9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="P9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2000000000000002</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="Q9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2</v>
+        <v>1.9</v>
       </c>
       <c r="R9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3</v>
+        <v>0.5</v>
       </c>
       <c r="S9" s="28" t="s">
         <v>145</v>
@@ -6106,19 +6112,19 @@
       </c>
       <c r="H10" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>2.2999999999999998</v>
+        <v>4.8</v>
       </c>
       <c r="I10" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1</v>
+        <v>1.4</v>
       </c>
       <c r="J10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9</v>
+        <v>3.1</v>
       </c>
       <c r="K10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2999999999999998</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="L10" s="28">
         <f t="shared" ca="1" si="0"/>
@@ -6126,27 +6132,27 @@
       </c>
       <c r="M10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7</v>
+        <v>0.8</v>
       </c>
       <c r="N10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4</v>
+        <v>4.8</v>
       </c>
       <c r="O10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>0.3</v>
       </c>
       <c r="P10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1</v>
+        <v>3.5</v>
       </c>
       <c r="Q10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.3</v>
+        <v>1.4</v>
       </c>
       <c r="R10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7</v>
+        <v>3.6</v>
       </c>
       <c r="S10" s="28" t="s">
         <v>153</v>
@@ -6298,47 +6304,47 @@
       </c>
       <c r="H13">
         <f t="shared" ref="H13:R18" ca="1" si="3">ROUND(RAND()*5,1)</f>
-        <v>1.7</v>
+        <v>3.9</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="3"/>
-        <v>4.5999999999999996</v>
+        <v>3.9</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="3"/>
-        <v>4.9000000000000004</v>
+        <v>0.2</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="3"/>
-        <v>0.1</v>
+        <v>3.9</v>
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="3"/>
-        <v>1.2</v>
+        <v>0.3</v>
       </c>
       <c r="M13">
         <f t="shared" ca="1" si="3"/>
-        <v>0.9</v>
+        <v>4.5</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="3"/>
-        <v>4.0999999999999996</v>
+        <v>4.7</v>
       </c>
       <c r="O13">
         <f t="shared" ca="1" si="3"/>
-        <v>2.8</v>
+        <v>4.8</v>
       </c>
       <c r="P13">
         <f t="shared" ca="1" si="3"/>
-        <v>1.9</v>
+        <v>3.2</v>
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="3"/>
-        <v>0.1</v>
+        <v>1.2</v>
       </c>
       <c r="R13">
         <f t="shared" ca="1" si="3"/>
-        <v>0.2</v>
+        <v>3.4</v>
       </c>
       <c r="S13" s="37" t="s">
         <v>144</v>
@@ -6368,47 +6374,47 @@
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="3"/>
-        <v>4.2</v>
+        <v>0.3</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="3"/>
-        <v>4.3</v>
+        <v>3</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>2.9</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="3"/>
-        <v>3.2</v>
+        <v>1.3</v>
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="3"/>
-        <v>0.2</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="M14">
         <f t="shared" ca="1" si="3"/>
-        <v>1.7</v>
+        <v>1.8</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="3"/>
-        <v>1.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="O14">
         <f t="shared" ca="1" si="3"/>
-        <v>1.6</v>
+        <v>3.8</v>
       </c>
       <c r="P14">
         <f t="shared" ca="1" si="3"/>
-        <v>0.5</v>
+        <v>2.9</v>
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="3"/>
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="R14">
         <f t="shared" ca="1" si="3"/>
-        <v>2.2999999999999998</v>
+        <v>2.6</v>
       </c>
       <c r="S14" t="s">
         <v>147</v>
@@ -6438,47 +6444,47 @@
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="3"/>
-        <v>3.1</v>
+        <v>2.1</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="3"/>
-        <v>1.3</v>
+        <v>2.5</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="3"/>
-        <v>3.9</v>
+        <v>0.7</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3.6</v>
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="3"/>
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="M15">
         <f t="shared" ca="1" si="3"/>
-        <v>0.3</v>
+        <v>4.3</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="3"/>
-        <v>4.0999999999999996</v>
+        <v>0.1</v>
       </c>
       <c r="O15">
         <f t="shared" ca="1" si="3"/>
-        <v>1.1000000000000001</v>
+        <v>2.5</v>
       </c>
       <c r="P15">
         <f t="shared" ca="1" si="3"/>
-        <v>3.8</v>
+        <v>4.7</v>
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="R15">
         <f t="shared" ca="1" si="3"/>
-        <v>1.5</v>
+        <v>4.8</v>
       </c>
       <c r="S15" t="s">
         <v>145</v>
@@ -6509,47 +6515,47 @@
       <c r="G16" s="17"/>
       <c r="H16" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>0.6</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="3"/>
-        <v>2.6</v>
+        <v>4.8</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="3"/>
-        <v>4.8</v>
+        <v>1.8</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="3"/>
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="3"/>
-        <v>1.1000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="M16">
         <f t="shared" ca="1" si="3"/>
-        <v>1.5</v>
+        <v>2.9</v>
       </c>
       <c r="N16">
         <f t="shared" ca="1" si="3"/>
-        <v>2.5</v>
+        <v>1.2</v>
       </c>
       <c r="O16">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>2.8</v>
       </c>
       <c r="P16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.4</v>
+        <v>1.5</v>
       </c>
       <c r="Q16">
         <f t="shared" ca="1" si="3"/>
-        <v>2.5</v>
+        <v>1.6</v>
       </c>
       <c r="R16">
         <f t="shared" ca="1" si="3"/>
-        <v>3.2</v>
+        <v>4.7</v>
       </c>
       <c r="S16" s="18" t="s">
         <v>152</v>
@@ -6579,47 +6585,47 @@
       </c>
       <c r="H17" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="3"/>
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="3"/>
-        <v>4.3</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="3"/>
-        <v>4.3</v>
+        <v>2.7</v>
       </c>
       <c r="L17">
         <f t="shared" ca="1" si="3"/>
-        <v>2.2999999999999998</v>
+        <v>3.4</v>
       </c>
       <c r="M17">
         <f t="shared" ca="1" si="3"/>
-        <v>0.7</v>
+        <v>1.2</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="3"/>
-        <v>3.1</v>
+        <v>2.7</v>
       </c>
       <c r="O17">
         <f t="shared" ca="1" si="3"/>
-        <v>3.8</v>
+        <v>2</v>
       </c>
       <c r="P17">
         <f t="shared" ca="1" si="3"/>
-        <v>1.8</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="Q17">
         <f t="shared" ca="1" si="3"/>
-        <v>4.4000000000000004</v>
+        <v>3.6</v>
       </c>
       <c r="R17">
         <f t="shared" ca="1" si="3"/>
-        <v>0.8</v>
+        <v>1.9</v>
       </c>
       <c r="S17" s="18" t="s">
         <v>152</v>
@@ -6649,47 +6655,47 @@
       </c>
       <c r="H18" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>0.7</v>
+        <v>1.6</v>
       </c>
       <c r="I18" s="18">
-        <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>1.5</v>
+        <f t="shared" ref="I18:R18" ca="1" si="4">ROUND(RAND()*5,1)</f>
+        <v>4.8</v>
       </c>
       <c r="J18" s="18">
-        <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>4.5</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.1</v>
       </c>
       <c r="K18" s="18">
-        <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>2.8</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
       </c>
       <c r="L18" s="18">
-        <f ca="1">ROUND(RAND()*5,1)</f>
+        <f t="shared" ca="1" si="4"/>
+        <v>4.8</v>
+      </c>
+      <c r="M18" s="18">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="N18" s="18">
+        <f t="shared" ca="1" si="4"/>
         <v>2.2000000000000002</v>
       </c>
-      <c r="M18" s="18">
-        <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>0.1</v>
-      </c>
-      <c r="N18" s="18">
-        <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>1.9</v>
-      </c>
       <c r="O18" s="18">
-        <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>4.9000000000000004</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>3.2</v>
       </c>
       <c r="P18" s="18">
-        <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>4.5999999999999996</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>2.6</v>
       </c>
       <c r="Q18" s="18">
-        <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>0.7</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>4.2</v>
       </c>
       <c r="R18" s="18">
-        <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>4.4000000000000004</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
       </c>
       <c r="S18" s="18" t="s">
         <v>152</v>
@@ -6992,19 +6998,19 @@
     <cfRule type="duplicateValues" dxfId="33" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:G1">
-    <cfRule type="duplicateValues" dxfId="32" priority="52"/>
-    <cfRule type="duplicateValues" dxfId="31" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:K1">
-    <cfRule type="duplicateValues" dxfId="30" priority="21"/>
-    <cfRule type="duplicateValues" dxfId="29" priority="23"/>
-    <cfRule type="duplicateValues" dxfId="28" priority="24"/>
-    <cfRule type="duplicateValues" dxfId="27" priority="25"/>
-    <cfRule type="duplicateValues" dxfId="26" priority="26"/>
-    <cfRule type="duplicateValues" dxfId="25" priority="30"/>
-    <cfRule type="duplicateValues" dxfId="24" priority="31"/>
-    <cfRule type="duplicateValues" dxfId="23" priority="34"/>
-    <cfRule type="duplicateValues" dxfId="22" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1">
     <cfRule type="duplicateValues" dxfId="21" priority="37"/>
@@ -7013,13 +7019,13 @@
     <cfRule type="duplicateValues" dxfId="20" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB1:AC1">
-    <cfRule type="duplicateValues" dxfId="19" priority="20"/>
-    <cfRule type="duplicateValues" dxfId="18" priority="22"/>
-    <cfRule type="duplicateValues" dxfId="17" priority="27"/>
-    <cfRule type="duplicateValues" dxfId="16" priority="28"/>
-    <cfRule type="duplicateValues" dxfId="15" priority="29"/>
-    <cfRule type="duplicateValues" dxfId="14" priority="33"/>
-    <cfRule type="duplicateValues" dxfId="13" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC1">
     <cfRule type="duplicateValues" dxfId="12" priority="19"/>

</xml_diff>